<commit_message>
added and modified rules
</commit_message>
<xml_diff>
--- a/Чек-лист для Литеры-7 (в каскаде 5.4.6.210) обновленный.xlsx
+++ b/Чек-лист для Литеры-7 (в каскаде 5.4.6.210) обновленный.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\p.larionov\Desktop\Документы\Тестовая документация\Литера 7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{30022A9B-2C73-4C6C-818E-816FCAF79588}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B4F2289-97B9-4443-BD49-89C6A94911D6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{CD4BA97D-4515-4BB2-A9C3-2E9FA8DA9E3C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="222">
   <si>
     <t>Результат</t>
   </si>
@@ -464,12 +464,6 @@
     <t>тут используется группа индексов  нужно сделать на "Р" такие же тесты</t>
   </si>
   <si>
-    <t>Поиск по КС по правилу "Т СНГ" с одной ошибкой в ФИО</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу "Т СНГ" с одной ошибкой, в одной компоненте ФИГ</t>
-  </si>
-  <si>
     <t>Поиск по КС по правилу "В СНГ" с одной ошибкой в ФИО</t>
   </si>
   <si>
@@ -508,18 +502,6 @@
     <t>Проверка поиска по КС в "Каскад" по правилу с индексом "С" с двумя ошибками, в двух компонентах ФИГ</t>
   </si>
   <si>
-    <t>Поиск по КС по правилу "З-Н ЕВРОПЕЙЦЫ" с двумя ошибками в ФИО</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу "З-Н ЕВРОПЕЙЦЫ" с двумя ошибками, в одной компоненте ФИГ</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "З-Н РФ" с двумя ошибками, в ФИО</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу "З-Н РФ" с двумя ошибками, в двух компонентах ФИГ</t>
-  </si>
-  <si>
     <t>Поиск по КС по правилу "С СНГ" с двумя ошибками, в ФИО</t>
   </si>
   <si>
@@ -536,81 +518,15 @@
 Пассажир брался из БД pakdb таблица OU_List</t>
   </si>
   <si>
-    <t>Поиск по КС по правилу "К-Р АЗИЯ" с двумя ошибками, в ФИО</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу "К-Р АЗИЯ" с двумя ошибками, в одной компоненте ФИГ</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "Т СОСТАВНЫЕ" с двумя ошибками в ФИО</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу "Т СОСТАВНЫЕ" с двумя ошибками, в одной компоненте ФИГ</t>
-  </si>
-  <si>
-    <t>Индекс у пассажира Т для стран группы "СОСТАВНЫЕ"
-Пассажир брался из БД pakdb таблица OU_List</t>
-  </si>
-  <si>
     <t>Поиск по КС по правилу "Т ЕВРОПЕЙЦЫ" с двумя ошибками в ФИО</t>
   </si>
   <si>
     <t>Проверка поиска по КС в "Каскад" по правилу "Т ЕВРОПЕЙЦЫ" с двумя ошибками, в одной компоненте ФИГ</t>
   </si>
   <si>
-    <t>Поиск по КС по правилу "В АЗИЯ" с двумя ошибками в ФИО</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу "В АЗИЯ" с двумя ошибками, в одной компоненте ФИГ</t>
-  </si>
-  <si>
     <t>Перестановка именных компанент</t>
   </si>
   <si>
-    <t>Поиск по КС по правилу "К-Р СОСТАВНЫЕ" с перестановкой компонент</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу "К-Р СОСТАВНЫЕ" с перестановкой именных компонент местами</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "З-Н СОСТАВНЫЕ" с перестановкой компонент</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу "З-Н СОСТАВНЫЕ" с перестановкой именных компонент местами</t>
-  </si>
-  <si>
-    <t>Индекс у пассажира З или Н для стран группы "СОСТАВНЫЕ"
-Пассажир брался из БД pakdb таблица OU_List</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "Т СОСТАВНЫЕ" с перестановкой компонент</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу "Т СОСТАВНЫЕ" с перестановкой именных компонент местами</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "Ф СОСТАВНЫЕ" с перестановкой компонент</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу "Ф СОСТАВНЫЕ" с перестановкой именных компонент местами</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "В СОСТАВНЫЕ" с перестановкой компонент</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу "В СОСТАВНЫЕ" с перестановкой именных компонент местами</t>
-  </si>
-  <si>
-    <t>Индекс у пассажира В для стран группы "СОСТАВНЫЕ"
-Пассажир брался из БД pakdb таблица OU_List</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "Т РФ" с перестановкой компонент</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу "Т РФ" с перестановкой именных компонент местами</t>
-  </si>
-  <si>
     <t>Не совпадение с первой компанентой ФИО</t>
   </si>
   <si>
@@ -620,128 +536,206 @@
     <t>Проверка поиска по КС в "Каскад" по правилу "Т РФ" с замененной первой компонентой ФИО на другую</t>
   </si>
   <si>
-    <t>Поиск по КС по правилу "Т СНГ" с заменой первой компоненты</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу "Т СНГ" с замененной первой компонентой ФИО на другую</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "Т ЕВРОПЕЙЦЫ" с заменой первой компоненты</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу "Т ЕВРОПЕЙЦЫ" с замененной первой компонентой ФИО на другую</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "Т АЗИЯ" с заменой первой компоненты</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу "Т АЗИЯ" с замененной первой компонентой ФИО на другую</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "В СНГ" с заменой первой компоненты</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу "В СНГ" с замененной первой компонентой ФИО на другую</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "В ЕВРОПЕЙЦЫ" с заменой первой компоненты</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу "В ЕВРОПЕЙЦЫ" с замененной первой компонентой ФИО на другую</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "В АЗИЯ" с заменой первой компоненты</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу "В АЗИЯ" с замененной первой компонентой ФИО на другую</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "К-Р СОСТАВНЫЕ"с заменой первой компоненты</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу "К-Р СОСТАВНЫЕ" с замененной первой компонентой ФИО на другую</t>
-  </si>
-  <si>
     <t>Отсутствие любой компоненты ФИО</t>
   </si>
   <si>
-    <t>Поиск по КС по правилу "К-Р РФ" с одной компонентой ФИО</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу "К-Р РФ" с одной компонентой ФИО, две компоненты удалить</t>
-  </si>
-  <si>
-    <t>Индекс у пассажира К или Р для страны группы "РФ"
-Пассажир брался из БД pakdb таблица OU_List</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "З-Н СНГ" с одной компонентами ФИО</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу "З-Н СНГ" с одной  компонентой ФИО, две компоненты удалить</t>
-  </si>
-  <si>
-    <t>Индекс у пассажира З или Н для стран группы "СНГ"
-Пассажир брался из БД pakdb таблица OU_List</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "Т АЗИЯ" с одной компонентой ФИО</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу "Т АЗИЯ" с одной  компонентой ФИО, две компоненты удалить</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "Ф ЕВРОПЕЙЦЫ" с одной компонентой ФИО</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу "Ф ЕВРОПЕЙЦЫ" с одной компонентой ФИО, две компоненты удалить</t>
-  </si>
-  <si>
-    <t>Индекс у пассажира Ф для стран группы "ЕВРОПЕЙЦЫ"
-Пассажир брался из БД pakdb таблица OU_List</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "С СОСТАВНЫЕ" с двумя компонентами ФИО</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу "С СОСТАВНЫЕ" с двумя  компонентами ФИО, одну из компонент удалить</t>
-  </si>
-  <si>
-    <t>Индекс у пассажира С для стран группы "СОСТАВНЫЕ"
-Пассажир брался из БД pakdb таблица OU_List</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "В СНГ" с двумя компонентами ФИО</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу "В СНГ" с двумя  компонентами ФИО, одну из компонент удалить</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "З-Н РФ" с одной компонентой ФИО</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу "З-Н РФ" с одной компонентой ФИО, две компоненты удалить</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "Ф АЗИЯ" с двумя компонентами ФИО</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу "Ф АЗИЯ" с двумя компонентами ФИО, одну компоненту удалить</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "Т ЕВРОПЕЙЦЫ" с двумя компонентами ФИО</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу "Т ЕВРОПЕЙЦЫ" с двумя компонентами ФИО, одну компоненту удалить</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "З-Н СОСТАВНЫЕ" с одной компонентой ФИО</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу "З-Н СОСТАВНЫЕ" с одной  компонентой ФИО, две компоненты удалить</t>
-  </si>
-  <si>
     <t>Название тест-кейса</t>
+  </si>
+  <si>
+    <t>Поиск по КС по правилу c  индексом "З" с двумя ошибками в ФИО</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" по правилу с индексом "З" с двумя ошибками, в одной компоненте ФИГ</t>
+  </si>
+  <si>
+    <t>Индекс у пассажира З "ЕВРОПЕЙЦЫ"
+Пассажир брался из БД pakdb таблица OU_List</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" по правилу с индексом "З" с двумя ошибками, в двух компонентах ФИГ</t>
+  </si>
+  <si>
+    <t>Поиск по КС по правилу с индексом "З" с двумя ошибками, в ФИО</t>
+  </si>
+  <si>
+    <t>Поиск по КС по правилу с индексом "Р" с двумя ошибками, в ФИО</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" по правилу с индексом "Р" с двумя ошибками, в одной компоненте ФИГ</t>
+  </si>
+  <si>
+    <t>Индекс у пассажира Р
+Пассажир брался из БД pakdb таблица OU_List</t>
+  </si>
+  <si>
+    <t>Поиск по КС по правилу c индексом "Т" с одной ошибкой в ФИО</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" по правилу с индексом "Т" с одной ошибкой, в одной компоненте ФИГ</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" по правилу с индексом "Т" с двумя ошибками, в одной компоненте ФИГ</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" по правилу с индексом "В" с двумя ошибками, в одной компоненте ФИГ</t>
+  </si>
+  <si>
+    <t>Поиск по КС по правилу "К" с перестановкой компонент</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" по правилу "К" с перестановкой именных компонент местами</t>
+  </si>
+  <si>
+    <t>Поиск по КС по правилу "Р" с перестановкой компонент</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" по правилу "Р" с перестановкой именных компонент местами</t>
+  </si>
+  <si>
+    <t>Поиск по КС по правилу "З" с перестановкой компонент</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" по правилу "З" с перестановкой именных компонент местами</t>
+  </si>
+  <si>
+    <t>Поиск по КС по правилу "Н" с перестановкой компонент</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" по правилу "Н" с перестановкой именных компонент местами</t>
+  </si>
+  <si>
+    <t>Поиск по КС по правилу "Т" с перестановкой компонент</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" по правилу "Т" с перестановкой именных компонент местами</t>
+  </si>
+  <si>
+    <t>Поиск по КС по правилу "Ф" с перестановкой компонент</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" по правилу "Ф" с перестановкой именных компонент местами</t>
+  </si>
+  <si>
+    <t>Поиск по КС по правилу "В" с перестановкой компонент</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" по правилу "В" с перестановкой именных компонент местами</t>
+  </si>
+  <si>
+    <t>Поиск по КС по правилу "Т" с заменой первой компоненты</t>
+  </si>
+  <si>
+    <t>Поиск по КС по правилу "П" с заменой первой компоненты</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" по правилу "Т" с замененной первой компонентой ФИО на другую</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" по правилу "П" с замененной первой компонентой ФИО на другую</t>
+  </si>
+  <si>
+    <t>Поиск по КС по правилу "Д" с заменой первой компоненты</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" по правилу "Д" с замененной первой компонентой ФИО на другую</t>
+  </si>
+  <si>
+    <t>Индекс у пассажира Д 
+Пассажир брался из БД pakdb таблица OU_List</t>
+  </si>
+  <si>
+    <t>Поиск по КС по правилу "В" с заменой первой компоненты</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" по правилу "В" с замененной первой компонентой ФИО на другую</t>
+  </si>
+  <si>
+    <t>Поиск по КС по правилу "З" с заменой первой компоненты</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" по правилу "З" с замененной первой компонентой ФИО на другую</t>
+  </si>
+  <si>
+    <t>Поиск по КС по правилу Н" с заменой первой компоненты</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" по правилу "Н" с замененной первой компонентой ФИО на другую</t>
+  </si>
+  <si>
+    <t>Поиск по КС по правилу "Р"с заменой первой компоненты</t>
+  </si>
+  <si>
+    <t>Поиск по КС по правилу "К"с заменой первой компоненты</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" по правилу "К" с замененной первой компонентой ФИО на другую</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" по правилу "Р" с замененной первой компонентой ФИО на другую</t>
+  </si>
+  <si>
+    <t>Индекс у пассажира  Р
+Пассажир брался из БД pakdb таблица OU_List</t>
+  </si>
+  <si>
+    <t>Поиск по КС по правилу "К" с одной компонентой ФИО</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" по правилу "К" с одной компонентой ФИО, две компоненты удалить</t>
+  </si>
+  <si>
+    <t>Поиск по КС по правилу "Р" с одной компонентой ФИО</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" по правилу "Р" с одной компонентой ФИО, две компоненты удалить</t>
+  </si>
+  <si>
+    <t>Поиск по КС по правилу "Н" с одной компонентами ФИО</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" по правилу "Н" с одной  компонентой ФИО, две компоненты удалить</t>
+  </si>
+  <si>
+    <t>Поиск по КС по правилу "З" с одной компонентами ФИО</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" по правилу "З" с одной  компонентой ФИО, две компоненты удалить</t>
+  </si>
+  <si>
+    <t>Поиск по КС по правилу "Т" с одной компонентой ФИО</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" по правилу "Т" с одной  компонентой ФИО, две компоненты удалить</t>
+  </si>
+  <si>
+    <t>Поиск по КС по правилу "Ф" с одной компонентой ФИО</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" по правилу "Ф" с одной компонентой ФИО, две компоненты удалить</t>
+  </si>
+  <si>
+    <t>Поиск по КС по правилу "Т" с двумя компонентами ФИО</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" по правилу "Т" с двумя компонентами ФИО, одну компоненту удалить</t>
+  </si>
+  <si>
+    <t>Поиск по КС по правилу "Ф" с двумя компонентами ФИО</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" по правилу "Ф" с двумя компонентами ФИО, одну компоненту удалить</t>
+  </si>
+  <si>
+    <t>Поиск по КС по правилу "С" с двумя компонентами ФИО</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" по правилу "С" с двумя  компонентами ФИО, одну из компонент удалить</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" по правилу "В" с двумя  компонентами ФИО, одну из компонент удалить</t>
+  </si>
+  <si>
+    <t>Поиск по КС по правилу "В" с двумя компонентами ФИО</t>
   </si>
 </sst>
 </file>
@@ -835,7 +829,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -868,6 +862,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1184,24 +1182,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB07023A-D923-4003-9F9B-F5C7C3A05B81}">
-  <dimension ref="A1:E90"/>
+  <dimension ref="A1:I90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="E88" sqref="E88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28" customWidth="1"/>
+    <col min="1" max="1" width="30.85546875" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
     <col min="3" max="3" width="27" customWidth="1"/>
     <col min="4" max="4" width="28.7109375" customWidth="1"/>
     <col min="5" max="5" width="33.28515625" customWidth="1"/>
+    <col min="6" max="6" width="27.28515625" customWidth="1"/>
+    <col min="7" max="7" width="19.42578125" customWidth="1"/>
+    <col min="8" max="8" width="32.85546875" customWidth="1"/>
+    <col min="9" max="9" width="25.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>222</v>
+        <v>157</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1213,7 +1215,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1839,27 +1841,25 @@
       </c>
     </row>
     <row r="50" spans="1:5" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="B50" s="9"/>
-      <c r="C50" s="10" t="s">
-        <v>134</v>
-      </c>
-      <c r="D50" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="E50" s="11" t="s">
-        <v>119</v>
-      </c>
+      <c r="A50" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="B50" s="6"/>
+      <c r="C50" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="D50" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E50" s="13"/>
     </row>
     <row r="51" spans="1:5" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B51" s="9"/>
       <c r="C51" s="10" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D51" s="10" t="s">
         <v>55</v>
@@ -1870,35 +1870,35 @@
     </row>
     <row r="52" spans="1:5" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B52" s="3"/>
       <c r="C52" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B53" s="3"/>
       <c r="C53" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="87" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="8" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B54" s="9"/>
       <c r="C54" s="10" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D54" s="10" t="s">
         <v>50</v>
@@ -1909,62 +1909,66 @@
     </row>
     <row r="55" spans="1:5" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B55" s="3"/>
       <c r="C55" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="96" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="B56" s="3"/>
-      <c r="C56" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>44</v>
-      </c>
+      <c r="A56" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B56" s="6"/>
+      <c r="C56" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="D56" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="E56" s="13"/>
     </row>
     <row r="57" spans="1:5" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>149</v>
+        <v>162</v>
       </c>
       <c r="B57" s="3"/>
       <c r="C57" s="2" t="s">
-        <v>150</v>
+        <v>161</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>70</v>
+        <v>18</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="B58" s="3"/>
-      <c r="C58" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="D58" s="2" t="s">
+      <c r="A58" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="B58" s="9"/>
+      <c r="C58" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="D58" s="10" t="s">
         <v>88</v>
+      </c>
+      <c r="E58" s="11" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="8" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="B59" s="9"/>
       <c r="C59" s="10" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="D59" s="10" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="E59" s="11" t="s">
         <v>119</v>
@@ -1972,239 +1976,264 @@
     </row>
     <row r="60" spans="1:5" ht="97.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="B60" s="3"/>
       <c r="C60" s="2" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>73</v>
+        <v>165</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
-        <v>158</v>
+        <v>105</v>
       </c>
       <c r="B61" s="3"/>
       <c r="C61" s="2" t="s">
-        <v>159</v>
+        <v>168</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>160</v>
+        <v>107</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="B62" s="3"/>
-      <c r="C62" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="D62" s="2" t="s">
+      <c r="A62" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="B62" s="9"/>
+      <c r="C62" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="D62" s="10" t="s">
         <v>47</v>
       </c>
+      <c r="E62" s="12"/>
     </row>
     <row r="63" spans="1:5" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>163</v>
+        <v>114</v>
       </c>
       <c r="B63" s="3"/>
       <c r="C63" s="2" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>58</v>
+        <v>33</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
     </row>
-    <row r="65" spans="1:4" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B65" s="3"/>
       <c r="C65" s="2" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="G65" s="3"/>
+      <c r="H65" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="I65" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="B66" s="3"/>
       <c r="C66" s="2" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" ht="105" customHeight="1" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="F66" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="G66" s="3"/>
+      <c r="H66" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="I66" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="B67" s="3"/>
       <c r="C67" s="2" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="B68" s="3"/>
       <c r="C68" s="2" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" ht="105" customHeight="1" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="B69" s="3"/>
       <c r="C69" s="2" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" ht="81" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="2" t="s">
-        <v>178</v>
-      </c>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" ht="81" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="2"/>
       <c r="B70" s="3"/>
-      <c r="C70" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="D70" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C70" s="2"/>
+      <c r="D70" s="2"/>
+    </row>
+    <row r="71" spans="1:9" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>180</v>
+        <v>153</v>
       </c>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
     </row>
-    <row r="72" spans="1:4" ht="81" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" ht="81" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>181</v>
+        <v>154</v>
       </c>
       <c r="B72" s="3"/>
       <c r="C72" s="2" t="s">
-        <v>182</v>
+        <v>155</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B73" s="3"/>
       <c r="C73" s="2" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>185</v>
       </c>
       <c r="B74" s="3"/>
       <c r="C74" s="2" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B75" s="3"/>
       <c r="C75" s="2" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B76" s="3"/>
       <c r="C76" s="2" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B77" s="3"/>
       <c r="C77" s="2" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B78" s="3"/>
       <c r="C78" s="2" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="B79" s="3"/>
       <c r="C79" s="2" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="F79" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="G79" s="3"/>
+      <c r="H79" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="I79" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>197</v>
+        <v>156</v>
       </c>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
@@ -2212,122 +2241,122 @@
     </row>
     <row r="81" spans="1:4" ht="97.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="B81" s="3"/>
       <c r="C81" s="2" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>200</v>
+        <v>137</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
-        <v>201</v>
+        <v>208</v>
       </c>
       <c r="B82" s="3"/>
       <c r="C82" s="2" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>203</v>
+        <v>18</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="B83" s="3"/>
       <c r="C83" s="2" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="96" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="B84" s="3"/>
       <c r="C84" s="2" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>208</v>
+        <v>110</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
-        <v>209</v>
+        <v>218</v>
       </c>
       <c r="B85" s="3"/>
       <c r="C85" s="2" t="s">
-        <v>210</v>
+        <v>219</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>211</v>
+        <v>30</v>
       </c>
     </row>
     <row r="86" spans="1:4" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
-        <v>212</v>
+        <v>221</v>
       </c>
       <c r="B86" s="3"/>
       <c r="C86" s="2" t="s">
-        <v>213</v>
+        <v>220</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>55</v>
+        <v>33</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="B87" s="3"/>
       <c r="C87" s="2" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>70</v>
+        <v>27</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B88" s="3"/>
       <c r="C88" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>64</v>
+        <v>24</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
       <c r="B89" s="3"/>
       <c r="C89" s="2" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>47</v>
+        <v>201</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="102" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="B90" s="3"/>
       <c r="C90" s="2" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>211</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ended file check list of M1
</commit_message>
<xml_diff>
--- a/Чек-лист для Литеры-7 (в каскаде 5.4.6.210) обновленный.xlsx
+++ b/Чек-лист для Литеры-7 (в каскаде 5.4.6.210) обновленный.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\p.larionov\Desktop\Документы\Тестовая документация\Литера 7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B4F2289-97B9-4443-BD49-89C6A94911D6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC1B4239-3FE2-4757-B146-6114418B3ECF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{CD4BA97D-4515-4BB2-A9C3-2E9FA8DA9E3C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="227">
   <si>
     <t>Результат</t>
   </si>
@@ -530,12 +530,6 @@
     <t>Не совпадение с первой компанентой ФИО</t>
   </si>
   <si>
-    <t>Поиск по КС по правилу "Т РФ" с заменой первой компоненты</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу "Т РФ" с замененной первой компонентой ФИО на другую</t>
-  </si>
-  <si>
     <t>Отсутствие любой компоненты ФИО</t>
   </si>
   <si>
@@ -736,13 +730,34 @@
   </si>
   <si>
     <t>Поиск по КС по правилу "В" с двумя компонентами ФИО</t>
+  </si>
+  <si>
+    <t>нужно обдумать об количестве компонент с ошибками</t>
+  </si>
+  <si>
+    <t>Тест почти пройден</t>
+  </si>
+  <si>
+    <t>с РФ выдал ответ поиска хотя не должен тест не пройден</t>
+  </si>
+  <si>
+    <t xml:space="preserve">с РФ не выдает ответ поиска тест не пройден </t>
+  </si>
+  <si>
+    <t xml:space="preserve">нужно написать тесты для нескольких стран для РФ отдельные тесты по сути все тесты которые тут есть будут дублироваться </t>
+  </si>
+  <si>
+    <t>Поиск по КС по правилу с индексом "С"</t>
+  </si>
+  <si>
+    <t>Поиск по КС по правилу с индексом "В"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -781,6 +796,14 @@
       <family val="1"/>
       <charset val="204"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFFC000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -802,7 +825,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -825,11 +848,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -866,6 +900,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1184,8 +1224,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB07023A-D923-4003-9F9B-F5C7C3A05B81}">
   <dimension ref="A1:I90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="E88" sqref="E88"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1203,7 +1243,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1227,19 +1267,26 @@
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3"/>
+      <c r="B3" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>6</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="3"/>
+      <c r="B4" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
@@ -1251,7 +1298,9 @@
       <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="3"/>
+      <c r="B5" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="C5" s="2" t="s">
         <v>11</v>
       </c>
@@ -1263,7 +1312,9 @@
       <c r="A6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="3"/>
+      <c r="B6" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="C6" s="2" t="s">
         <v>14</v>
       </c>
@@ -1275,7 +1326,9 @@
       <c r="A7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="3"/>
+      <c r="B7" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="C7" s="2" t="s">
         <v>17</v>
       </c>
@@ -1287,7 +1340,9 @@
       <c r="A8" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="3"/>
+      <c r="B8" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="C8" s="2" t="s">
         <v>20</v>
       </c>
@@ -1299,7 +1354,9 @@
       <c r="A9" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="3"/>
+      <c r="B9" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="C9" s="2" t="s">
         <v>23</v>
       </c>
@@ -1311,7 +1368,9 @@
       <c r="A10" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="3"/>
+      <c r="B10" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="C10" s="2" t="s">
         <v>26</v>
       </c>
@@ -1321,9 +1380,11 @@
     </row>
     <row r="11" spans="1:5" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" s="3"/>
+        <v>225</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="C11" s="2" t="s">
         <v>29</v>
       </c>
@@ -1333,9 +1394,11 @@
     </row>
     <row r="12" spans="1:5" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" s="6"/>
+        <v>226</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="C12" s="7" t="s">
         <v>32</v>
       </c>
@@ -1652,43 +1715,60 @@
       <c r="A35" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B35" s="3"/>
+      <c r="B35" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="C35" s="2" t="s">
         <v>94</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>95</v>
+      </c>
+      <c r="E35" s="11" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="81" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B36" s="3"/>
+      <c r="B36" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="C36" s="2" t="s">
         <v>97</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>6</v>
+      </c>
+      <c r="E36" s="11" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B37" s="3"/>
+      <c r="B37" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="C37" s="2" t="s">
         <v>99</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" ht="127.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
+      <c r="E37" s="11" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="97.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B38" s="3"/>
+      <c r="B38" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="C38" s="2" t="s">
         <v>102</v>
       </c>
@@ -1700,7 +1780,9 @@
       <c r="A39" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="B39" s="3"/>
+      <c r="B39" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="C39" s="2" t="s">
         <v>104</v>
       </c>
@@ -1712,7 +1794,9 @@
       <c r="A40" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="B40" s="3"/>
+      <c r="B40" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="C40" s="2" t="s">
         <v>106</v>
       </c>
@@ -1724,7 +1808,9 @@
       <c r="A41" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="B41" s="3"/>
+      <c r="B41" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="C41" s="2" t="s">
         <v>109</v>
       </c>
@@ -1736,7 +1822,9 @@
       <c r="A42" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="B42" s="3"/>
+      <c r="B42" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="C42" s="2" t="s">
         <v>112</v>
       </c>
@@ -1748,7 +1836,9 @@
       <c r="A43" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="B43" s="3"/>
+      <c r="B43" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="C43" s="2" t="s">
         <v>115</v>
       </c>
@@ -1775,7 +1865,9 @@
       <c r="A45" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="B45" s="3"/>
+      <c r="B45" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="C45" s="2" t="s">
         <v>121</v>
       </c>
@@ -1787,7 +1879,9 @@
       <c r="A46" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="B46" s="3"/>
+      <c r="B46" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="C46" s="2" t="s">
         <v>123</v>
       </c>
@@ -1814,7 +1908,9 @@
       <c r="A48" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="B48" s="3"/>
+      <c r="B48" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="C48" s="2" t="s">
         <v>127</v>
       </c>
@@ -1829,7 +1925,9 @@
       <c r="A49" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="B49" s="3"/>
+      <c r="B49" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="C49" s="2" t="s">
         <v>131</v>
       </c>
@@ -1842,11 +1940,13 @@
     </row>
     <row r="50" spans="1:5" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="B50" s="6"/>
+        <v>164</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="C50" s="7" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D50" s="7" t="s">
         <v>24</v>
@@ -1872,7 +1972,9 @@
       <c r="A52" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="B52" s="3"/>
+      <c r="B52" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="C52" s="2" t="s">
         <v>136</v>
       </c>
@@ -1884,7 +1986,9 @@
       <c r="A53" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="B53" s="3"/>
+      <c r="B53" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="C53" s="2" t="s">
         <v>139</v>
       </c>
@@ -1911,7 +2015,9 @@
       <c r="A55" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="B55" s="3"/>
+      <c r="B55" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="C55" s="2" t="s">
         <v>144</v>
       </c>
@@ -1921,24 +2027,28 @@
     </row>
     <row r="56" spans="1:5" ht="96" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C56" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="D56" s="7" t="s">
         <v>158</v>
-      </c>
-      <c r="B56" s="6"/>
-      <c r="C56" s="7" t="s">
-        <v>159</v>
-      </c>
-      <c r="D56" s="7" t="s">
-        <v>160</v>
       </c>
       <c r="E56" s="13"/>
     </row>
     <row r="57" spans="1:5" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="B57" s="3"/>
+        <v>160</v>
+      </c>
+      <c r="B57" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="C57" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>18</v>
@@ -1976,23 +2086,27 @@
     </row>
     <row r="60" spans="1:5" ht="97.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="B60" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="D60" s="2" t="s">
         <v>163</v>
-      </c>
-      <c r="B60" s="3"/>
-      <c r="C60" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="B61" s="3"/>
+      <c r="B61" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="C61" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>107</v>
@@ -2015,9 +2129,11 @@
       <c r="A63" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="B63" s="3"/>
+      <c r="B63" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="C63" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>33</v>
@@ -2033,43 +2149,51 @@
     </row>
     <row r="65" spans="1:9" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="B65" s="3"/>
+        <v>168</v>
+      </c>
+      <c r="B65" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="C65" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>137</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="G65" s="3"/>
+        <v>170</v>
+      </c>
+      <c r="G65" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="H65" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="I65" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="66" spans="1:9" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="B66" s="3"/>
+        <v>172</v>
+      </c>
+      <c r="B66" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="C66" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>18</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="G66" s="3"/>
+        <v>174</v>
+      </c>
+      <c r="G66" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="H66" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="I66" s="2" t="s">
         <v>140</v>
@@ -2077,11 +2201,13 @@
     </row>
     <row r="67" spans="1:9" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="B67" s="3"/>
+        <v>176</v>
+      </c>
+      <c r="B67" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="C67" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>24</v>
@@ -2089,11 +2215,13 @@
     </row>
     <row r="68" spans="1:9" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="B68" s="3"/>
+        <v>178</v>
+      </c>
+      <c r="B68" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="C68" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>27</v>
@@ -2101,11 +2229,13 @@
     </row>
     <row r="69" spans="1:9" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="B69" s="3"/>
+        <v>180</v>
+      </c>
+      <c r="B69" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="C69" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>33</v>
@@ -2127,35 +2257,44 @@
     </row>
     <row r="72" spans="1:9" ht="81" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="B72" s="3"/>
+        <v>195</v>
+      </c>
+      <c r="B72" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="C72" s="2" t="s">
-        <v>155</v>
+        <v>198</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>67</v>
+        <v>199</v>
       </c>
     </row>
     <row r="73" spans="1:9" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B73" s="14" t="s">
+        <v>221</v>
+      </c>
+      <c r="C73" s="2" t="s">
         <v>184</v>
-      </c>
-      <c r="B73" s="3"/>
-      <c r="C73" s="2" t="s">
-        <v>186</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>107</v>
       </c>
+      <c r="E73" s="15" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="74" spans="1:9" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="B74" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C74" s="2" t="s">
         <v>185</v>
-      </c>
-      <c r="B74" s="3"/>
-      <c r="C74" s="2" t="s">
-        <v>187</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>6</v>
@@ -2163,23 +2302,27 @@
     </row>
     <row r="75" spans="1:9" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B75" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="D75" s="2" t="s">
         <v>188</v>
-      </c>
-      <c r="B75" s="3"/>
-      <c r="C75" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="D75" s="2" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="76" spans="1:9" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="B76" s="3"/>
+        <v>189</v>
+      </c>
+      <c r="B76" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="C76" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D76" s="2" t="s">
         <v>33</v>
@@ -2187,23 +2330,30 @@
     </row>
     <row r="77" spans="1:9" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="B77" s="3"/>
+        <v>191</v>
+      </c>
+      <c r="B77" s="14" t="s">
+        <v>221</v>
+      </c>
       <c r="C77" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D77" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="E77" s="15" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="78" spans="1:9" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="B78" s="3"/>
+        <v>193</v>
+      </c>
+      <c r="B78" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="C78" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D78" s="2" t="s">
         <v>21</v>
@@ -2211,29 +2361,21 @@
     </row>
     <row r="79" spans="1:9" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="B79" s="3"/>
+        <v>196</v>
+      </c>
+      <c r="B79" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="C79" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D79" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F79" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="G79" s="3"/>
-      <c r="H79" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="I79" s="2" t="s">
-        <v>201</v>
-      </c>
     </row>
     <row r="80" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
@@ -2241,11 +2383,13 @@
     </row>
     <row r="81" spans="1:4" ht="97.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
-        <v>202</v>
-      </c>
-      <c r="B81" s="3"/>
+        <v>200</v>
+      </c>
+      <c r="B81" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="C81" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D81" s="2" t="s">
         <v>137</v>
@@ -2253,11 +2397,13 @@
     </row>
     <row r="82" spans="1:4" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
-        <v>208</v>
-      </c>
-      <c r="B82" s="3"/>
+        <v>206</v>
+      </c>
+      <c r="B82" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="C82" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D82" s="2" t="s">
         <v>18</v>
@@ -2265,11 +2411,13 @@
     </row>
     <row r="83" spans="1:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
-        <v>210</v>
-      </c>
-      <c r="B83" s="3"/>
+        <v>208</v>
+      </c>
+      <c r="B83" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="C83" s="2" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D83" s="2" t="s">
         <v>24</v>
@@ -2277,11 +2425,13 @@
     </row>
     <row r="84" spans="1:4" ht="96" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="B84" s="3"/>
+        <v>210</v>
+      </c>
+      <c r="B84" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="C84" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D84" s="2" t="s">
         <v>110</v>
@@ -2289,11 +2439,13 @@
     </row>
     <row r="85" spans="1:4" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
-        <v>218</v>
-      </c>
-      <c r="B85" s="3"/>
+        <v>216</v>
+      </c>
+      <c r="B85" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="C85" s="2" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D85" s="2" t="s">
         <v>30</v>
@@ -2301,11 +2453,13 @@
     </row>
     <row r="86" spans="1:4" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
-        <v>221</v>
-      </c>
-      <c r="B86" s="3"/>
+        <v>219</v>
+      </c>
+      <c r="B86" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="C86" s="2" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D86" s="2" t="s">
         <v>33</v>
@@ -2313,11 +2467,13 @@
     </row>
     <row r="87" spans="1:4" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
-        <v>216</v>
-      </c>
-      <c r="B87" s="3"/>
+        <v>214</v>
+      </c>
+      <c r="B87" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="C87" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D87" s="2" t="s">
         <v>27</v>
@@ -2325,11 +2481,13 @@
     </row>
     <row r="88" spans="1:4" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="B88" s="3"/>
+        <v>212</v>
+      </c>
+      <c r="B88" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="C88" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D88" s="2" t="s">
         <v>24</v>
@@ -2337,23 +2495,27 @@
     </row>
     <row r="89" spans="1:4" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
-        <v>204</v>
-      </c>
-      <c r="B89" s="3"/>
+        <v>202</v>
+      </c>
+      <c r="B89" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="C89" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="102" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
-        <v>206</v>
-      </c>
-      <c r="B90" s="3"/>
+        <v>204</v>
+      </c>
+      <c r="B90" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="C90" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D90" s="2" t="s">
         <v>21</v>
@@ -2361,5 +2523,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added test case of added test case of
</commit_message>
<xml_diff>
--- a/Чек-лист для Литеры-7 (в каскаде 5.4.6.210) обновленный.xlsx
+++ b/Чек-лист для Литеры-7 (в каскаде 5.4.6.210) обновленный.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\p.larionov\Desktop\Документы\Тестовая документация\Литера 7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B865130D-86FF-499F-8C9D-F325643DF44E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63D2F2FC-6AFA-4218-9139-7661939251AC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{CD4BA97D-4515-4BB2-A9C3-2E9FA8DA9E3C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="299">
   <si>
     <t>Результат</t>
   </si>
@@ -94,125 +94,44 @@
 Пассажир брался из БД pakdb таблица OU_List</t>
   </si>
   <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу с индексом "Д" с двумя ошибкой, в одной компоненте ФИГ</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу с индексом "Т" с двумя ошибками, в двух компонентах ФИГ</t>
-  </si>
-  <si>
     <t>Индекс у пассажира Т 
 Пассажир брался из БД pakdb таблица OU_List</t>
   </si>
   <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу с индексом "Ф" с одной ошибкой, в двух компонентах ФИГ</t>
-  </si>
-  <si>
     <t>Индекс у пассажира Ф 
 Пассажир брался из БД pakdb таблица OU_List</t>
   </si>
   <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу с индексом "С" с одной ошибкой, в трех компонентеах ФИГ</t>
-  </si>
-  <si>
     <t>Индекс у пассажира С 
 Пассажир брался из БД pakdb таблица OU_List</t>
   </si>
   <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу с индексом "В" с двумя ошибками, в двух компонентах ФИГ</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу с индексом "С" с двумя ошибками, в одной компоненте ФИГ</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу синдексом "Ф" с двумя ошибками, в трех компонентах ФИГ</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу с индексом "З" с одной ошибкой, в трех компонентах ФИГ</t>
-  </si>
-  <si>
     <t>Индекс у пассажира З 
 Пассажир брался из БД pakdb таблица OU_List</t>
   </si>
   <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу с индексом "К" с двумя ошибками, в двух компонентах ФИГ</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу с индексом "К" с двумя ошибками, в трех компонентах ФИГ</t>
-  </si>
-  <si>
     <t>Индекс у пассажира К 
 Пассажир брался из БД pakdb таблица OU_List</t>
   </si>
   <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу с индексом "Н" с двумя ошибками, в одной компоненте ФИГ</t>
-  </si>
-  <si>
     <t>Индекс у пассажира Н 
 Пассажир брался из БД pakdb таблица OU_List</t>
   </si>
   <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу "Ф РФ" с двумя ошибками, в одной компоненте ФИГ</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу с индексом "С" с двумя ошибками, в двух компонентах ФИГ</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу "С СНГ" с двумя ошибками, в одной компоненте ФИГ</t>
-  </si>
-  <si>
     <t>Перестановка именных компанент</t>
   </si>
   <si>
     <t>Название тест-кейса</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу с индексом "З" с двумя ошибками, в одной компоненте ФИГ</t>
   </si>
   <si>
     <t>Индекс у пассажира З "ЕВРОПЕЙЦЫ"
 Пассажир брался из БД pakdb таблица OU_List</t>
   </si>
   <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу с индексом "З" с двумя ошибками, в двух компонентах ФИГ</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу с индексом "Р" с двумя ошибками, в одной компоненте ФИГ</t>
-  </si>
-  <si>
     <t>Индекс у пассажира Р
 Пассажир брался из БД pakdb таблица OU_List</t>
   </si>
   <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу с индексом "Т" с одной ошибкой, в одной компоненте ФИГ</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу с индексом "Т" с двумя ошибками, в одной компоненте ФИГ</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу с индексом "В" с двумя ошибками, в одной компоненте ФИГ</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу "К" с перестановкой именных компонент местами</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу "Р" с перестановкой именных компонент местами</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу "З" с перестановкой именных компонент местами</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу "Н" с перестановкой именных компонент местами</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу "Т" с перестановкой именных компонент местами</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу "Ф" с перестановкой именных компонент местами</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу "В" с перестановкой именных компонент местами</t>
-  </si>
-  <si>
     <t>Индекс у пассажира Д 
 Пассажир брался из БД pakdb таблица OU_List</t>
   </si>
@@ -221,479 +140,23 @@
 Пассажир брался из БД pakdb таблица OU_List</t>
   </si>
   <si>
-    <t>Поиск по КС по правилу с индексом "В", для страны РФ</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу с индексом "С" для страны РФ</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу с индексом "К" для страны РФ</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу с индексом "Р" для страны РФ</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу с индексом "З" для страны РФ</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу с индексом "Т" для страны РФ</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу с индексом "Н" для страны РФ</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу с индексом "Ф"  для страны РФ</t>
-  </si>
-  <si>
     <t>Индекс у пассажира В 
 Пассажир брался из БД pakdb таблица OU_List</t>
   </si>
   <si>
-    <t>Проверка поиска по контрольнуму списку (КС) в "Каскад" по правилу с индексом "П", без ошибок в Фамильно-именной группе(ФИГ)</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу с индексом "Д", без ошибок в ФИГ</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу с индексом "К", без ошибок в ФИГ</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу с индексом "Р", без ошибок в ФИГ</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу с индексом "З", без ошибок в ФИГ</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу с индексом "Н", без ошибок в ФИГ</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу с индексом "Т", без ошибок в ФИГ</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу с индексом "Ф", без ошибок в ФИГ</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу с индексом "С", без ошибок в ФИГ</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу с индексом "В", без ошибок в ФИГ</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу с индексом"Т", без ошибок в ФИГ</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу "Ф", без ошибок в ФИГ</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу с индексом "Д" с одной ошибкой, в одной компоненте ФИГ</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу с индексом "П" с двумя ошибками в ФИГ, в трех компонентах</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу с индексом "П" с одной ошибкой в ФИГ, в двух компонентах</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу с индексом "П" с двумя ошибками в ФИГ, в одной компоненте</t>
-  </si>
-  <si>
     <t>Поиск по КС ошибками в ФИГ</t>
   </si>
   <si>
-    <t>Поиск по КС по правилу  с индексом "Д" для страны Туркмения</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу с индексом "К" для страны Узбекистан</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу с индексом "З"  для страны Грузия</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу с индексом "Р"  для страны Армения</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу с индексом "Н"  для страны Таджикистан</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу с индексом "Ф"  для страны Казахстан</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу с индексом "С" для страны Китай</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу с индексом "В" для страны Украина</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу с индексом "В" для страны США</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу с индексом "С" для страны Польша</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу с индексом "Т" для страны Азербайджан</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу с индексом "Ф" для страны Литва</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу с индексом "Т" для страны Финляндия</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу с индексом "К" для страны Германия</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу с индексом "Р" для страны Перу</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу с индексом "З" для страны Бразилия</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу с индексом "Ф" для страны Тунис</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу индексом "С" для страны Египет</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу с индексом "В" для страны Австралия</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу с индексом "П" с двумя ошибками в ФИГ для страны РФ</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "Д"с одна ошибкой в ФИГ для страны РФ</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу с индексом "Д"с двумя ошибками в ФИГ для страны РФ</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу с индексом "Т" с двумя ошибками в ФИГ для страны РФ</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу с индексом "Ф" с одной ошибкой в ФИГ для страны РФ</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу сиднексом "С" с одной ошибкой в ФИГ для страны РФ</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу с индексом "В" с двумя ошибками в ФИГ для страны РФ</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу с идексом "С" с двумя ошибками в ФИГ для страны РФ</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Поиск по КС по правилу с индексом "Ф" с двумя ошибками в ФИГ для страны РФ</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу с индексом "З"с одной ошибкой в ФИГ для страны РФ</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу с индексом "К" с двумя ошибками в ФИГ для страны РФ</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу c индексом "Т" с одной ошибкой в ФИГ для страны РФ</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу с индексом "Р" с двумя ошибками в ФИГ для страны РФ</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу с индексом "Н" с двумя ошибками в ФИГ для страны РФ</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу с индексом "С" с двумя ошибками, в ФИГ для страны РФ</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу c  индексом "З" с двумя ошибками в ФИГ для страны РФ</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу с индексом "З" с двумя ошибками, в ФИГ для страны РФ</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу с индексом "Р" с двумя ошибками, в ФИГ для страны РФ</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу с индексом "П" с одной ошибкой в ФИГ для страны Латвия</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу с индексом "П" с двумя ошибками в ФИГ для страны Туркмения</t>
-  </si>
-  <si>
     <t>Поиск по контрольнуму списку пассажира с индексом "П" для страны Эстония</t>
   </si>
   <si>
-    <t>Поиск по КС по правилу с индексом "П" с двумя ошибками в ФИГ для страны Азербайджан</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Поиск по КС по правилу "Д" с одной ошибкой в ФИГ для страны Таджикистан </t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу с индексом "Д"с двумя ошибками в ФИГ для страны Франция</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу с индексом "Т" с двумя ошибками в ФИГ для страны Армения</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу с индексом "Ф" с одной ошибкой в ФИГ для страны Люксенбург</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу сиднексом "С" с одной ошибкой в ФИГ для страны Алжир</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу с индексом "В" с двумя ошибками в ФИГ для страны Ангола</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "В" с двумя ошибками в ФИГ для страны ЮАР</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу с идексом "С" с двумя ошибками в ФИГ для страны ОАЭ</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу "В" с двумя ошибками, в трех компонентах ФИГ</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Поиск по КС по правилу с индексом "Ф" с двумя ошибками в ФИГ для страны Индия</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу с индексом "З"с одной ошибкой в ФИГ для страны Тайвань, провинция Китая</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу с индексом "К" с двумя ошибками в ФИГ для страны Вьетнам</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу c индексом "Т" с одной ошибкой в ФИГ для страны Узбекистан</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу с индексом "В" с одной ошибкой в ФИГ для страны Украина</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу "В" с одной ошибкой, в одной компоненте ФИГ</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу с индексом "Т" с двумя ошибками, в трех компонентах ФИГ</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу с индексом "Т" с двумя ошибками в ФИГ  для страны Индонезия</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу с индексом "Р" с двумя ошибками в ФИГ для страны Израиль</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу с индексом "Н" с двумя ошибками в ФИГ для страны Иран</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "Ф" с двумя ошибками, в ФИГ для страны Афганистан</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу с индексом "С" с двумя ошибками, в ФИГ для страны Турция</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу c  индексом "З" с двумя ошибками в ФИГ для страны Греция</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу с индексом "З" с двумя ошибками, в ФИГ для страны Румыния</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "С" с двумя ошибками, в ФИГ для страны Албания</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу "Ф" с двумя ошибками, в одной компоненте ФИГ</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "Ф" с двумя ошибками, в ФИГ для страны Черногория</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу с индексом "Н" с одной ошибкой, в трех компонентах ФИГ</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу с индексом "Р" с двумя ошибками, в двух компонентах ФИГ</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу с индексом "Р" с двумя ошибками, в ФИГ для страны Бахрейн</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу с индексом "Т" с двумя ошибками в ФИГ для страны Багамы</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу с индексом "В" с двумя ошибками в ФИГ для страны Гибралтар</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу с индексом "Н"с одной ошибкой в ФИГ для страны Испания</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу с индексом "Р" с двумя ошибками в ФИГ для страны Монголия</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Поиск по КС по правилу с индексом "П" с одной ошибкой в ФИГ для страны РФ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Поиск по КС по правилу "Ф" с перестановкой компонент для страны </t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "К" с перестановкой компонент для страны РФ</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "З" с перестановкой компонент для страны РФ</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "Т" с перестановкой компонент для страны РФ</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "Ф" с перестановкой компонент для страны РФ</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "В" с перестановкой компонент для страны РФ</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "Р" с перестановкой компонент для страны РФ</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "Н" с перестановкой компонент для страны РФ</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "К" с перестановкой компонент для страны Таджикистан</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "З" с перестановкой компонент для страны Индия</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "Т" с перестановкой компонент для страны Китай</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "В" с перестановкой компонент для страны Италия</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "Р" с перестановкой компонент для страны Мексика</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "Н" с перестановкой компонент для страны Аргентина</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "Р"с заменой первой компоненты для страны РФ</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "Т" с заменой первой компоненты для страны РФ</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "П" с заменой первой компоненты для страны РФ</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "Д" с заменой первой компоненты для страны РФ</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "В" с заменой первой компоненты для страны РФ</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "З" с заменой первой компоненты для страны РФ</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу Н" с заменой первой компоненты для страны РФ</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "К"с заменой первой компоненты для страны РФ</t>
-  </si>
-  <si>
     <t>Тест не пройден</t>
   </si>
   <si>
     <t>Не совпадение с первой компанентой ФИГ</t>
   </si>
   <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу "Р" с замененной первой компонентой ФИГ на другую</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу "Т" с замененной первой компонентой ФИГ на другую</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу "П" с замененной первой компонентой ФИГ на другую</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу "Д" с замененной первой компонентой ФИГ на другую</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу "В" с замененной первой компонентой ФИГ на другую</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу "З" с замененной первой компонентой ФИГ на другую</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу "Н" с замененной первой компонентой ФИГ на другую</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу "К" с замененной первой компонентой ФИГ на другую</t>
-  </si>
-  <si>
     <t>Отсутствие любой компоненты ФИГ</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу "К" с одной компонентой ФИГ, две компоненты удалить</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу "З" с одной  компонентой ФИГ, две компоненты удалить</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу "Т" с одной  компонентой ФИГ, две компоненты удалить</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу "Ф" с одной компонентой ФИГ, две компоненты удалить</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу "С" с двумя  компонентами ФИГ, одну из компонент удалить</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу "В" с двумя  компонентами ФИГ, одну из компонент удалить</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу "Ф" с двумя компонентами ФИГ, одну компоненту удалить</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу "Т" с двумя компонентами ФИГ, одну компоненту удалить</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу "Р" с одной компонентой ФИГ, две компоненты удалить</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу "Н" с одной  компонентой ФИГ, две компоненты удалить</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "Р" с заменой первой компоненты для страны Грузия</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "Т" с заменой первой компоненты для страны Чехия</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "П" с заменой первой компоненты для страны Норвегия</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "Д" с заменой первой компоненты для страны Малайзия</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "В" с заменой первой компоненты для страны Непал</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "З" с заменой первой компоненты для страны Узбекистан</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу Н" с заменой первой компоненты для страны Кипр</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "К"с заменой первой компоненты для страны Нигер</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "С" с заменой первой компоненты для страны РФ</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу "С" с замененной первой компонентой ФИГ на другую</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "Ф"с заменой первой компоненты для страны Марокко</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу "Ф" с замененной первой компонентой ФИГ на другую</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу "К" с замененной первой компонентой ФИГ на другую, ФИГ содержит четыре компоненты</t>
-  </si>
-  <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу "Д" с замененной первой компонентой ФИГ на другую, ФИГ содержит четыре компоненты</t>
   </si>
   <si>
     <t xml:space="preserve">Индекс у пассажира С
@@ -720,24 +183,6 @@
 В правилах к данному индексу запрещена замена первой компоненты   </t>
   </si>
   <si>
-    <t>Проверка поиска по КС в "Каскад" по правилу "Т" с замененной первой компонентой ФИГ на другую, ФИГ содержит четыре компоненты</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "Т"с заменой первой компоненты для страны РФ, ФИГ с четырьмя  компоненты</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "Р"с заменой первой компоненты для страны Коморы, ФИГ с четырьмя компоненты</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "В"с заменой первой компоненты для страны Буркина-Фасо, ФИГ с четырьмя компоненты</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "Д"с заменой первой компоненты для страны РФ, ФИГ с четырьмя компоненты</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "К"с заменой первой компоненты для страны РФ, ФИГ с четырьмя компоненты</t>
-  </si>
-  <si>
     <t xml:space="preserve">Индекс у пассажира К
 Пассажир брался из БД pakdb таблица OU_List  
 В форме "Результат поиска" есть результат поиска 
@@ -756,64 +201,774 @@
 В правилах к данному индексу разрешена замена первой компоненты   </t>
   </si>
   <si>
-    <t>Поиск по КС по правилу "К" с одной компонентой ФИГ для страны Швеция</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "К" с одной компонентой ФИГ для страны РФ</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "З" с одной компонентами ФИГ для страны РФ</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "Т" с одной компонентой ФИГ для страны РФ</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "Ф" с одной компонентой ФИГ для страны РФ</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "С" с двумя компонентами ФИГ для страны РФ</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "В" с двумя компонентами ФИГ для страны РФ</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "Ф" с двумя компонентами ФИГ для страны РФ</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "Т" с двумя компонентами ФИГ для страны РФ</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "Р" с одной компонентой ФИГ для страны РФ</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "Н" с одной компонентами ФИГ для страны РФ</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "З" с одной компонентами ФИГ для страны Дания</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "Т" с одной компонентой ФИГ для страны Бурунди</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "Ф" с одной компонентой ФИГ для страны Конго</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "С" с двумя компонентами ФИГ для страны Франция</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "В" с двумя компонентами ФИГ для страны Туркменистан</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "Ф" с двумя компонентами ФИГ для страны Уганда</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "Т" с двумя компонентами ФИГ для страны Сент-Винсент и Гренадины</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "Р" с одной компонентой ФИГ для страны Соломоновы острова</t>
-  </si>
-  <si>
-    <t>Поиск по КС по правилу "Н" с одной компонентами ФИГ для страны Гамбия</t>
+    <t>Поиск по КС пассажира  с индексом "Д" для страны Туркмения</t>
+  </si>
+  <si>
+    <t>Поиск по КС пассажира с индексом "К" для страны Узбекистан</t>
+  </si>
+  <si>
+    <t>Поиск по КС пассажира с индексом "Р"  для страны Армения</t>
+  </si>
+  <si>
+    <t>Поиск по КС пассажира с индексом "З"  для страны Грузия</t>
+  </si>
+  <si>
+    <t>Поиск по КС пассажира с индексом "Н"  для страны Таджикистан</t>
+  </si>
+  <si>
+    <t>Поиск по КС пассажира с индексом "Т" для страны Азербайджан</t>
+  </si>
+  <si>
+    <t>Поиск по КС пассажира с индексом "Ф"  для страны Казахстан</t>
+  </si>
+  <si>
+    <t>Поиск по КС пассажира с индексом "С" для страны Китай</t>
+  </si>
+  <si>
+    <t>Поиск по КС пассажира с индексом "В" для страны Украина</t>
+  </si>
+  <si>
+    <t>Поиск по КС пассажира с индексом "С" для страны РФ</t>
+  </si>
+  <si>
+    <t>Поиск по КС пассажира с индексом "К" для страны РФ</t>
+  </si>
+  <si>
+    <t>Поиск по КС пассажира с индексом "З" для страны РФ</t>
+  </si>
+  <si>
+    <t>Поиск по КС пассажира с индексом "Т" для страны РФ</t>
+  </si>
+  <si>
+    <t>Поиск по КС пассажира с индексом "Ф"  для страны РФ</t>
+  </si>
+  <si>
+    <t>Поиск по КС пассажира с индексом "Н" для страны РФ</t>
+  </si>
+  <si>
+    <t>Поиск по КС пассажира с индексом "С" для страны Польша</t>
+  </si>
+  <si>
+    <t>Поиск по КС пассажира с индексом "В" для страны США</t>
+  </si>
+  <si>
+    <t>Поиск по КС пассажира с индексом "Ф" для страны Литва</t>
+  </si>
+  <si>
+    <t>Поиск по КС пассажира с индексом "К" для страны Германия</t>
+  </si>
+  <si>
+    <t>Поиск по КС пассажира с индексом "Р" для страны Перу</t>
+  </si>
+  <si>
+    <t>Поиск по КС пассажира с индексом "З" для страны Бразилия</t>
+  </si>
+  <si>
+    <t>Поиск по КС пассажира с индексом "Ф" для страны Тунис</t>
+  </si>
+  <si>
+    <t>Поиск по КС пассажира индексом "С" для страны Египет</t>
+  </si>
+  <si>
+    <t>Поиск по КС пассажира с индексом "В" для страны Австралия</t>
+  </si>
+  <si>
+    <t>Поиск по КС пассажира c индексом "Т" с одной ошибкой в ФИГ для страны Узбекистан</t>
+  </si>
+  <si>
+    <t>Проверка поиска по контрольнуму списку (КС) в "Каскад" пассажира с индексом с индексом "П", без ошибок в Фамильно-именной группе(ФИГ)</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом с индексом "Д", без ошибок в ФИГ</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом с индексом "К", без ошибок в ФИГ</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом с индексом "Р", без ошибок в ФИГ</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом с индексом "З", без ошибок в ФИГ</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом с индексом "Н", без ошибок в ФИГ</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом с индексом "Т", без ошибок в ФИГ</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом с индексом "Ф", без ошибок в ФИГ</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом с индексом "С", без ошибок в ФИГ</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом с индексом "В", без ошибок в ФИГ</t>
+  </si>
+  <si>
+    <t>Поиск по КС пассажира с индексом с индексом "В", для страны РФ</t>
+  </si>
+  <si>
+    <t>Поиск по КС пассажира с индексом с индексом "Р" для страны РФ</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом с индексом"Т", без ошибок в ФИГ</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом "Ф", без ошибок в ФИГ</t>
+  </si>
+  <si>
+    <t>Поиск по КС пассажира с индексом с индексом "Т" для страны Финляндия</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом с индексом "П" с одной ошибкой в ФИГ, в двух компонентах</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом с индексом "П" с двумя ошибками в ФИГ, в трех компонентах</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом с индексом "П" с двумя ошибками в ФИГ, в одной компоненте</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом с индексом "Д" с одной ошибкой, в одной компоненте ФИГ</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом с индексом "Д" с двумя ошибкой, в одной компоненте ФИГ</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом с индексом "Т" с двумя ошибками, в двух компонентах ФИГ</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом с индексом "Ф" с одной ошибкой, в двух компонентах ФИГ</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом с индексом "С" с одной ошибкой, в трех компонентеах ФИГ</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом с индексом "В" с двумя ошибками, в двух компонентах ФИГ</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом "В" с двумя ошибками, в трех компонентах ФИГ</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом с индексом "С" с двумя ошибками, в одной компоненте ФИГ</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом синдексом "Ф" с двумя ошибками, в трех компонентах ФИГ</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом с индексом "Т" с двумя ошибками, в трех компонентах ФИГ</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом с индексом "З" с одной ошибкой, в трех компонентах ФИГ</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом с индексом "К" с двумя ошибками, в двух компонентах ФИГ</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом с индексом "Т" с одной ошибкой, в одной компоненте ФИГ</t>
+  </si>
+  <si>
+    <t>Поиск по КС пассажира с индексом с индексом "В" с одной ошибкой в ФИГ для страны Украина</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом "В" с одной ошибкой, в одной компоненте ФИГ</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом с индексом "К" с двумя ошибками, в трех компонентах ФИГ</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом с индексом "Н" с двумя ошибками, в одной компоненте ФИГ</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом "Ф РФ" с двумя ошибками, в одной компоненте ФИГ</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом с индексом "С" с двумя ошибками, в двух компонентах ФИГ</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом с индексом "З" с двумя ошибками, в одной компоненте ФИГ</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом с индексом "З" с двумя ошибками, в двух компонентах ФИГ</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом "С СНГ" с двумя ошибками, в одной компоненте ФИГ</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом "Ф" с двумя ошибками, в одной компоненте ФИГ</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом с индексом "Р" с двумя ошибками, в одной компоненте ФИГ</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом с индексом "Т" с двумя ошибками, в одной компоненте ФИГ</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом с индексом "В" с двумя ошибками, в одной компоненте ФИГ</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом с индексом "Н" с одной ошибкой, в трех компонентах ФИГ</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом с индексом "Р" с двумя ошибками, в двух компонентах ФИГ</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом "К" с перестановкой именных компонент местами</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом "З" с перестановкой именных компонент местами</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом "Т" с перестановкой именных компонент местами</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом "Ф" с перестановкой именных компонент местами</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом "В" с перестановкой именных компонент местами</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом "Р" с перестановкой именных компонент местами</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом "Н" с перестановкой именных компонент местами</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом "Р" с замененной первой компонентой ФИГ на другую</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом "Т" с замененной первой компонентой ФИГ на другую</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом "П" с замененной первой компонентой ФИГ на другую</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом "Д" с замененной первой компонентой ФИГ на другую</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом "В" с замененной первой компонентой ФИГ на другую</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом "З" с замененной первой компонентой ФИГ на другую</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом "Н" с замененной первой компонентой ФИГ на другую</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом "К" с замененной первой компонентой ФИГ на другую</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом "Ф" с замененной первой компонентой ФИГ на другую</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом "С" с замененной первой компонентой ФИГ на другую</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом "К" с замененной первой компонентой ФИГ на другую, ФИГ содержит четыре компоненты</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом "Д" с замененной первой компонентой ФИГ на другую, ФИГ содержит четыре компоненты</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом "Т" с замененной первой компонентой ФИГ на другую, ФИГ содержит четыре компоненты</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом "К" с одной компонентой ФИГ, две компоненты удалить</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом "З" с одной  компонентой ФИГ, две компоненты удалить</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом "Т" с одной  компонентой ФИГ, две компоненты удалить</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом "Ф" с одной компонентой ФИГ, две компоненты удалить</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом "С" с двумя  компонентами ФИГ, одну из компонент удалить</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом "В" с двумя  компонентами ФИГ, одну из компонент удалить</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом "Ф" с двумя компонентами ФИГ, одну компоненту удалить</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом "Т" с двумя компонентами ФИГ, одну компоненту удалить</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом "Р" с одной компонентой ФИГ, две компоненты удалить</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом "Н" с одной  компонентой ФИГ, две компоненты удалить</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом "К" с одним повторяющимся символом в одной компоненте ФИГ</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "Ф", с одной компонентой ФИГ для страны Конго</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "Т", с одной компонентой ФИГ для страны Бурунди</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "С", с двумя компонентами ФИГ для страны Франция</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "З", с одной компонентами ФИГ для страны Дания</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "В", с двумя компонентами ФИГ для страны Туркменистан</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "Ф", с двумя компонентами ФИГ для страны Уганда</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "Т", с двумя компонентами ФИГ для страны Сент-Винсент и Гренадины</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "Р", с одной компонентой ФИГ для страны Соломоновы острова</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "Н", с одной компонентами ФИГ для страны Гамбия</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "К", с одной компонентой ФИГ для страны РФ</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "З", с одной компонентами ФИГ для страны РФ</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "Т", с одной компонентой ФИГ для страны РФ</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "Ф", с одной компонентой ФИГ для страны РФ</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "С" с двумя компонентами ФИГ для страны РФ</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "В", с двумя компонентами ФИГ для страны РФ</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "Ф", с двумя компонентами ФИГ для страны РФ</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "Т", с двумя компонентами ФИГ для страны РФ</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "Р", с одной компонентой ФИГ для страны РФ</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "Н", с одной компонентами ФИГ для страны РФ</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом "Р" с двумя повторяющимися символами в двух компанентах ФИГ</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "К", с одним повторяющимся символом в ФИГ для страны РФ</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "Р", с двумя повторяющимися символами в ФИГ для страны РФ</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "З", с тремя повторяющимися символами в ФИГ для страны РФ</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом "З" с тремя повторяющимися символами в трех компонентах ФИГ</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "Н", с двумя повторяющимися символами в ФИГ для страны Камерун</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "Т", с  двумя повторяющимися символами в ФИГ для страны Габон</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом "Н" с тремя повторяющимися символами в одной компоненте ФИГ</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом "Т" с двумя повторяющимися символами в одной компоненте ФИГ</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "Ф", с одним повторяющимся символом в ФИГ для страны Йемен</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом "Ф" с одним повторяющимся символом в трех компонентах ФИГ</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом "С" с одним повторяющимся символом в двух компанентах ФИГ</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "С", с одним повторяющимся символом в ФИГ для страны Сент-Винсент и Гренадины</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "В", с двумя повторяющимися символами в ФИГ для страны Бутан</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом "В" с двумя повторяющимися символами в трех компонентах ФИГ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Поиск пассажира с индексом "В", с тремя повторяющимися символами в ФИГ для страны РФ </t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом "В" с тремя повторяющимися символами в двух компанентах ФИГ</t>
+  </si>
+  <si>
+    <t>Индекс у пассажира  В
+Пассажир брался из БД pakdb таблица OU_List</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Поиск пассажира с индексом "С", с тремя повторяющимися символами в ФИГ для страны РФ </t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом "С" с тремя повторяющимися символами  в трех компонентах ФИГ</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом "Ф" с тремя повторяющимися символами в двух компанентах ФИГ</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом "Т" с тремя повторяющимися символами в двух компанентах ФИГ</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом "Н" с тремя повторяющимися символами в двух компанентах ФИГ</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом "З" с одним повторяющимся символом в двух компанентах ФИГ</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "З", с одним повторяющимся символом в ФИГ для страны Гонконг</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "Н", с тремя повторяющимися символами в ФИГ для страны РФ</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "Т", с тремя повторяющимися символами в ФИГ для страны РФ</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "Ф", с одним повторяющимся символом в ФИГ для страны РФ</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "Р", с тремя повторяющимися символами в ФИГ для страны Мадагаскар</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом "Р" с тремя повторяющимися символами в трех компонентах ФИГ</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "К", с тремя повторяющимися символами в ФИГ для страны Того</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом "К" с тремя повторяющимися символами в двух компанентах ФИГ</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом "К" с двумя повторяющимися символами в трех компонентах ФИГ</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "Р", с одним повторяющимся символом в ФИГ для страны Уругвай</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом "Р" с одним повторяющимся символом в одной компоненте ФИГ</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "К", с двумя повторяющимися символами в ФИГ для страны Индия</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "З", с двумя повторяющимися символами в ФИГ для страны Уоллис и Футуна</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом "З" с двумя повторяющимися символами в одной компоненте ФИГ</t>
+  </si>
+  <si>
+    <t>Индекс у пассажира  З
+Пассажир брался из БД pakdb таблица OU_List</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом "Н" с двумя повторяющимися символами в одной компоненте ФИГ</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "Н", с двумя повторяющимися символами в ФИГ для страны Святая Елена</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "Т", с одним повторяющимся символом в ФИГ для страны Святая Елена</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом "Т" с одним повторяющимся символом в трех компонентах ФИГ</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "Ф", с двумя повторяющимися символами в ФИГ для страны Виргинские острова (США)</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом "Ф" с двумя повторяющимися символами в одной компоненте ФИГ</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом "С" с двумя повторяющимися символами в одной компоненте ФИГ</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "С", с двумя повторяющимися символами в ФИГ для страны Новая Каледония</t>
+  </si>
+  <si>
+    <t>Проверка поиска по КС в "Каскад" пассажира с индексом "В" с одним повторяющимся символом в одной компоненте ФИГ</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "В", с одним повторяющимся символом в ФИГ для страны Черногория</t>
+  </si>
+  <si>
+    <t>Добавление повторяющегося символа в любую компоненту ФИГ</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "К" с двумя ошибками в ФИГ для страны Вьетнам</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом с индексом "З"с одной ошибкой в ФИГ для страны Тайвань, провинция Китая</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "Т" с двумя ошибками в ФИГ  для страны Индонезия</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Поиск пассажира с индексом "Ф" с двумя ошибками в ФИГ для страны Индия</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с идексом "С" с двумя ошибками в ФИГ для страны ОАЭ</t>
+  </si>
+  <si>
+    <t>Поиск пассажира "В" с двумя ошибками в ФИГ для страны ЮАР</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "В" с двумя ошибками в ФИГ для страны Ангола</t>
+  </si>
+  <si>
+    <t>Поиск пассажира сиднексом "С" с одной ошибкой в ФИГ для страны Алжир</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "Ф" с одной ошибкой в ФИГ для страны Люксенбург</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "Т" с двумя ошибками в ФИГ для страны Армения</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "Д"с двумя ошибками в ФИГ для страны Франция</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Поиск пассажира "Д" с одной ошибкой в ФИГ для страны Таджикистан </t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "П" с двумя ошибками в ФИГ для страны Азербайджан</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "П" с двумя ошибками в ФИГ для страны Туркмения</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "П" с одной ошибкой в ФИГ для страны Латвия</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "Р" с двумя ошибками в ФИГ для страны Израиль</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "Н" с двумя ошибками в ФИГ для страны Иран</t>
+  </si>
+  <si>
+    <t>Поиск пассажира "Ф" с двумя ошибками, в ФИГ для страны Афганистан</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "С" с двумя ошибками, в ФИГ для страны Турция</t>
+  </si>
+  <si>
+    <t>Поиск пассажира c  индексом "З" с двумя ошибками в ФИГ для страны Греция</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "З" с двумя ошибками, в ФИГ для страны Румыния</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "С" с двумя ошибками, в ФИГ для страны Албания</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "Ф" с двумя ошибками, в ФИГ для страны Черногория</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "Р" с двумя ошибками, в ФИГ для страны Бахрейн</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "Т" с двумя ошибками в ФИГ для страны Багамы</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "В" с двумя ошибками в ФИГ для страны Гибралтар</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "Н"с одной ошибкой в ФИГ для страны Испания</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "Р" с двумя ошибками в ФИГ для страны Монголия</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Поиск пассажира с индексом "П" с одной ошибкой в ФИГ для страны РФ </t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "П" с двумя ошибками в ФИГ для страны РФ</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "Д"с одна ошибкой в ФИГ для страны РФ</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом с индексом "Д"с двумя ошибками в ФИГ для страны РФ</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "Т" с двумя ошибками в ФИГ для страны РФ</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "Ф" с одной ошибкой в ФИГ для страны РФ</t>
+  </si>
+  <si>
+    <t>Поиск пассажира сиднексом "С" с одной ошибкой в ФИГ для страны РФ</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "В" с двумя ошибками в ФИГ для страны РФ</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с идексом "С" с двумя ошибками в ФИГ для страны РФ</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Поиск пассажира с индексом "Ф" с двумя ошибками в ФИГ для страны РФ</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом с индексом "З"с одной ошибкой в ФИГ для страны РФ</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "К" с двумя ошибками в ФИГ для страны РФ</t>
+  </si>
+  <si>
+    <t>Поиск пассажира c индексом "Т" с одной ошибкой в ФИГ для страны РФ</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "Р" с двумя ошибками в ФИГ для страны РФ</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "Н" с двумя ошибками в ФИГ для страны РФ</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом с индексом "С" с двумя ошибками, в ФИГ для страны РФ</t>
+  </si>
+  <si>
+    <t>Поиск пассажира c  индексом "З" с двумя ошибками в ФИГ для страны РФ</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "З" с двумя ошибками, в ФИГ для страны РФ</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом с индексом "Р" с двумя ошибками, в ФИГ для страны РФ</t>
+  </si>
+  <si>
+    <t>Поиск пассажира "К", с перестановкой компонент для страны Таджикистан</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "З", с перестановкой компонент для страны Индия</t>
+  </si>
+  <si>
+    <t>Поиск пассажира "Т" с перестановкой компонент для страны Китай</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Поиск пассажира с индексом "Ф", с перестановкой компонент для страны </t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "В", с перестановкой компонент для страны Италия</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "Р", с перестановкой компонент для страны Мексика</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "Н", с перестановкой компонент для страны Аргентина</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "К" с перестановкой компонент для страны РФ</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "З" с перестановкой компонент для страны РФ</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "Т", с перестановкой компонент для страны РФ</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "Ф", с перестановкой компонент для страны РФ</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "В" с перестановкой компонент для страны РФ</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "Р", с перестановкой компонент для страны РФ</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "Н", с перестановкой компонент для страны РФ</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "Р", с заменой первой компоненты для страны Грузия</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "Т", с заменой первой компоненты для страны Чехия</t>
+  </si>
+  <si>
+    <t>Поиск пассажира  с индексом "П", с заменой первой компоненты для страны Норвегия</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "Д", с заменой первой компоненты для страны Малайзия</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "В", с заменой первой компоненты для страны Непал</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "З" с заменой первой компоненты для страны Узбекистан</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "Н", с заменой первой компоненты для страны Кипр</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "К", с заменой первой компоненты для страны Нигер</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "Ф", с заменой первой компоненты для страны Марокко</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "Р", с заменой первой компоненты для страны РФ</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "Т", с заменой первой компоненты для страны РФ</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "П", с заменой первой компоненты для страны РФ</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "Д", с заменой первой компоненты для страны РФ</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "В", с заменой первой компоненты для страны РФ</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "З", с заменой первой компоненты для страны РФ</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "Н", с заменой первой компоненты для страны РФ</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "К", с заменой первой компоненты для страны РФ</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "С", с заменой первой компоненты для страны РФ</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "К", с заменой первой компоненты для страны РФ, ФИГ с четырьмя компоненты</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "Д", с заменой первой компоненты для страны РФ, ФИГ с четырьмя компоненты</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "Т", с заменой первой компоненты для страны РФ, ФИГ с четырьмя  компоненты</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "Р"с заменой первой компоненты для страны Коморы, ФИГ с четырьмя компоненты</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "В", с заменой первой компоненты для страны Буркина-Фасо, ФИГ с четырьмя компоненты</t>
+  </si>
+  <si>
+    <t>Поиск пассажира с индексом "К", с одной компонентой ФИГ для страны Швеция</t>
   </si>
 </sst>
 </file>
@@ -1326,18 +1481,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB07023A-D923-4003-9F9B-F5C7C3A05B81}">
-  <dimension ref="A1:K143"/>
+  <dimension ref="A1:K168"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="A161" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A143" sqref="A143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.85546875" customWidth="1"/>
+    <col min="1" max="1" width="40.42578125" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="33.28515625" customWidth="1"/>
-    <col min="4" max="4" width="59.140625" customWidth="1"/>
+    <col min="3" max="3" width="43.140625" customWidth="1"/>
+    <col min="4" max="4" width="50.5703125" customWidth="1"/>
     <col min="5" max="5" width="33.28515625" customWidth="1"/>
     <col min="6" max="6" width="31.7109375" customWidth="1"/>
     <col min="7" max="7" width="19.42578125" customWidth="1"/>
@@ -1347,7 +1502,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1369,13 +1524,13 @@
     </row>
     <row r="3" spans="1:6" ht="99" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>122</v>
+        <v>32</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>4</v>
@@ -1384,13 +1539,13 @@
     </row>
     <row r="4" spans="1:6" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>83</v>
+        <v>43</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>5</v>
@@ -1398,13 +1553,13 @@
     </row>
     <row r="5" spans="1:6" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>84</v>
+        <v>44</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>6</v>
@@ -1413,27 +1568,27 @@
     </row>
     <row r="6" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>86</v>
+        <v>45</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>85</v>
+        <v>46</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>7</v>
@@ -1441,13 +1596,13 @@
     </row>
     <row r="8" spans="1:6" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>87</v>
+        <v>47</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>8</v>
@@ -1455,13 +1610,13 @@
     </row>
     <row r="9" spans="1:6" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>93</v>
+        <v>48</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>9</v>
@@ -1469,13 +1624,13 @@
     </row>
     <row r="10" spans="1:6" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>88</v>
+        <v>49</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>10</v>
@@ -1483,13 +1638,13 @@
     </row>
     <row r="11" spans="1:6" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>89</v>
+        <v>50</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>11</v>
@@ -1497,13 +1652,13 @@
     </row>
     <row r="12" spans="1:6" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>90</v>
+        <v>51</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>12</v>
@@ -1512,13 +1667,13 @@
     </row>
     <row r="13" spans="1:6" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>57</v>
+        <v>78</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>12</v>
@@ -1527,13 +1682,13 @@
     </row>
     <row r="14" spans="1:6" ht="78" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>11</v>
@@ -1542,13 +1697,13 @@
     </row>
     <row r="15" spans="1:6" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>6</v>
@@ -1557,28 +1712,28 @@
     </row>
     <row r="16" spans="1:6" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="E16" s="14"/>
     </row>
     <row r="17" spans="1:5" ht="81" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>7</v>
@@ -1587,13 +1742,13 @@
     </row>
     <row r="18" spans="1:5" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>9</v>
@@ -1602,13 +1757,13 @@
     </row>
     <row r="19" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>10</v>
@@ -1617,13 +1772,13 @@
     </row>
     <row r="20" spans="1:5" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>8</v>
@@ -1632,13 +1787,13 @@
     </row>
     <row r="21" spans="1:5" ht="81" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>92</v>
+        <v>58</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>11</v>
@@ -1647,58 +1802,58 @@
     </row>
     <row r="22" spans="1:5" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>91</v>
+        <v>59</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>65</v>
+        <v>30</v>
       </c>
       <c r="E22" s="14"/>
     </row>
     <row r="23" spans="1:5" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>94</v>
+        <v>60</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E23" s="14"/>
     </row>
     <row r="24" spans="1:5" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E24" s="14"/>
     </row>
     <row r="25" spans="1:5" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>96</v>
+        <v>61</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D25" s="6" t="s">
         <v>6</v>
@@ -1707,28 +1862,28 @@
     </row>
     <row r="26" spans="1:5" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>97</v>
+        <v>62</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="E26" s="14"/>
     </row>
     <row r="27" spans="1:5" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>98</v>
+        <v>63</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>7</v>
@@ -1737,28 +1892,28 @@
     </row>
     <row r="28" spans="1:5" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>99</v>
+        <v>64</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E28" s="14"/>
     </row>
     <row r="29" spans="1:5" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>100</v>
+        <v>65</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D29" s="6" t="s">
         <v>11</v>
@@ -1767,22 +1922,22 @@
     </row>
     <row r="30" spans="1:5" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>101</v>
+        <v>66</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>65</v>
+        <v>30</v>
       </c>
       <c r="E30" s="14"/>
     </row>
     <row r="31" spans="1:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>82</v>
+        <v>31</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -1791,13 +1946,13 @@
     </row>
     <row r="32" spans="1:5" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>120</v>
+        <v>228</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>16</v>
@@ -1806,13 +1961,13 @@
     </row>
     <row r="33" spans="1:9" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>121</v>
+        <v>227</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>4</v>
@@ -1821,13 +1976,13 @@
     </row>
     <row r="34" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>123</v>
+        <v>226</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>17</v>
@@ -1836,13 +1991,13 @@
     </row>
     <row r="35" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>124</v>
+        <v>225</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>5</v>
@@ -1851,13 +2006,13 @@
     </row>
     <row r="36" spans="1:9" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>125</v>
+        <v>224</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>18</v>
+        <v>87</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>5</v>
@@ -1865,55 +2020,55 @@
     </row>
     <row r="37" spans="1:9" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>126</v>
+        <v>223</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>19</v>
+        <v>88</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>127</v>
+        <v>222</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>21</v>
+        <v>89</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="69" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>128</v>
+        <v>221</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>23</v>
+        <v>90</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>129</v>
+        <v>220</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>25</v>
+        <v>91</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>12</v>
@@ -1921,13 +2076,13 @@
     </row>
     <row r="41" spans="1:9" ht="78" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="11" t="s">
-        <v>130</v>
+        <v>219</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>132</v>
+        <v>92</v>
       </c>
       <c r="D41" s="12" t="s">
         <v>12</v>
@@ -1940,44 +2095,44 @@
     </row>
     <row r="42" spans="1:9" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>131</v>
+        <v>218</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>26</v>
+        <v>93</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>133</v>
+        <v>217</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>27</v>
+        <v>94</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="11" t="s">
-        <v>140</v>
+        <v>216</v>
       </c>
       <c r="B44" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C44" s="12" t="s">
-        <v>139</v>
+        <v>95</v>
       </c>
       <c r="D44" s="12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E44" s="13"/>
       <c r="F44" s="18"/>
@@ -1987,16 +2142,16 @@
     </row>
     <row r="45" spans="1:9" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>134</v>
+        <v>215</v>
       </c>
       <c r="B45" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>28</v>
+        <v>96</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="E45" s="13"/>
       <c r="F45" s="20"/>
@@ -2006,13 +2161,13 @@
     </row>
     <row r="46" spans="1:9" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>135</v>
+        <v>214</v>
       </c>
       <c r="B46" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>30</v>
+        <v>97</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>6</v>
@@ -2025,13 +2180,13 @@
     </row>
     <row r="47" spans="1:9" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>136</v>
+        <v>67</v>
       </c>
       <c r="B47" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>45</v>
+        <v>98</v>
       </c>
       <c r="D47" s="6" t="s">
         <v>9</v>
@@ -2044,13 +2199,13 @@
     </row>
     <row r="48" spans="1:9" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="11" t="s">
-        <v>137</v>
+        <v>99</v>
       </c>
       <c r="B48" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C48" s="12" t="s">
-        <v>138</v>
+        <v>100</v>
       </c>
       <c r="D48" s="12" t="s">
         <v>12</v>
@@ -2063,41 +2218,41 @@
     </row>
     <row r="49" spans="1:9" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>141</v>
+        <v>229</v>
       </c>
       <c r="B49" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>31</v>
+        <v>101</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>142</v>
+        <v>230</v>
       </c>
       <c r="B50" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>33</v>
+        <v>102</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="11" t="s">
-        <v>143</v>
+        <v>231</v>
       </c>
       <c r="B51" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C51" s="12" t="s">
-        <v>35</v>
+        <v>103</v>
       </c>
       <c r="D51" s="12" t="s">
         <v>14</v>
@@ -2110,13 +2265,13 @@
     </row>
     <row r="52" spans="1:9" ht="78" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>144</v>
+        <v>232</v>
       </c>
       <c r="B52" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>36</v>
+        <v>104</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>11</v>
@@ -2124,28 +2279,28 @@
     </row>
     <row r="53" spans="1:9" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>145</v>
+        <v>233</v>
       </c>
       <c r="B53" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>40</v>
+        <v>105</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="E53" s="7"/>
     </row>
     <row r="54" spans="1:9" ht="87" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>146</v>
+        <v>234</v>
       </c>
       <c r="B54" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>42</v>
+        <v>106</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>7</v>
@@ -2153,13 +2308,13 @@
     </row>
     <row r="55" spans="1:9" ht="81" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="11" t="s">
-        <v>147</v>
+        <v>235</v>
       </c>
       <c r="B55" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C55" s="12" t="s">
-        <v>37</v>
+        <v>107</v>
       </c>
       <c r="D55" s="12" t="s">
         <v>15</v>
@@ -2172,13 +2327,13 @@
     </row>
     <row r="56" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="11" t="s">
-        <v>149</v>
+        <v>236</v>
       </c>
       <c r="B56" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C56" s="12" t="s">
-        <v>148</v>
+        <v>108</v>
       </c>
       <c r="D56" s="12" t="s">
         <v>10</v>
@@ -2191,41 +2346,41 @@
     </row>
     <row r="57" spans="1:9" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>152</v>
+        <v>237</v>
       </c>
       <c r="B57" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>43</v>
+        <v>109</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" ht="69" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>153</v>
+        <v>238</v>
       </c>
       <c r="B58" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>46</v>
+        <v>110</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="59" spans="1:9" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>154</v>
+        <v>239</v>
       </c>
       <c r="B59" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>47</v>
+        <v>111</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>12</v>
@@ -2236,43 +2391,43 @@
       <c r="H59" s="9"/>
       <c r="I59" s="9"/>
     </row>
-    <row r="60" spans="1:9" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>155</v>
+        <v>240</v>
       </c>
       <c r="B60" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>150</v>
+        <v>112</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>156</v>
+        <v>241</v>
       </c>
       <c r="B61" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>151</v>
+        <v>113</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>157</v>
+        <v>242</v>
       </c>
       <c r="B62" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>16</v>
@@ -2280,13 +2435,13 @@
     </row>
     <row r="63" spans="1:9" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>102</v>
+        <v>243</v>
       </c>
       <c r="B63" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>4</v>
@@ -2294,27 +2449,27 @@
     </row>
     <row r="64" spans="1:9" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>102</v>
+        <v>243</v>
       </c>
       <c r="B64" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>103</v>
+        <v>244</v>
       </c>
       <c r="B65" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>5</v>
@@ -2322,13 +2477,13 @@
     </row>
     <row r="66" spans="1:4" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
-        <v>104</v>
+        <v>245</v>
       </c>
       <c r="B66" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>18</v>
+        <v>87</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>5</v>
@@ -2336,111 +2491,111 @@
     </row>
     <row r="67" spans="1:4" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>105</v>
+        <v>246</v>
       </c>
       <c r="B67" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C67" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D68" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="D67" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="B68" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C68" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D68" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
-        <v>107</v>
+        <v>248</v>
       </c>
       <c r="B69" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>23</v>
+        <v>90</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" ht="81" customHeight="1" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
-        <v>108</v>
+        <v>249</v>
       </c>
       <c r="B70" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>25</v>
+        <v>91</v>
       </c>
       <c r="D70" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" ht="69" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
-        <v>109</v>
+        <v>250</v>
       </c>
       <c r="B71" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>26</v>
+        <v>93</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
-        <v>110</v>
+        <v>251</v>
       </c>
       <c r="B72" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>27</v>
+        <v>94</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
-        <v>111</v>
+        <v>252</v>
       </c>
       <c r="B73" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>28</v>
+        <v>96</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
-        <v>112</v>
+        <v>253</v>
       </c>
       <c r="B74" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>30</v>
+        <v>97</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>6</v>
@@ -2448,13 +2603,13 @@
     </row>
     <row r="75" spans="1:4" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
-        <v>113</v>
+        <v>254</v>
       </c>
       <c r="B75" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>45</v>
+        <v>98</v>
       </c>
       <c r="D75" s="6" t="s">
         <v>9</v>
@@ -2462,41 +2617,41 @@
     </row>
     <row r="76" spans="1:4" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="15" t="s">
-        <v>114</v>
+        <v>255</v>
       </c>
       <c r="B76" s="16" t="s">
         <v>13</v>
       </c>
       <c r="C76" s="17" t="s">
-        <v>31</v>
+        <v>101</v>
       </c>
       <c r="D76" s="17" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
-        <v>115</v>
+        <v>256</v>
       </c>
       <c r="B77" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>33</v>
+        <v>102</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
-        <v>116</v>
+        <v>257</v>
       </c>
       <c r="B78" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>36</v>
+        <v>104</v>
       </c>
       <c r="D78" s="2" t="s">
         <v>11</v>
@@ -2504,27 +2659,27 @@
     </row>
     <row r="79" spans="1:4" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
-        <v>117</v>
+        <v>258</v>
       </c>
       <c r="B79" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C79" s="6" t="s">
-        <v>40</v>
+        <v>105</v>
       </c>
       <c r="D79" s="6" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
-        <v>118</v>
+        <v>259</v>
       </c>
       <c r="B80" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>42</v>
+        <v>106</v>
       </c>
       <c r="D80" s="2" t="s">
         <v>7</v>
@@ -2532,41 +2687,41 @@
     </row>
     <row r="81" spans="1:11" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
-        <v>119</v>
+        <v>260</v>
       </c>
       <c r="B81" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>43</v>
+        <v>109</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
     </row>
     <row r="82" spans="1:11" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
-        <v>105</v>
+        <v>246</v>
       </c>
       <c r="B82" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>46</v>
+        <v>110</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="83" spans="1:11" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
-        <v>108</v>
+        <v>249</v>
       </c>
       <c r="B83" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>47</v>
+        <v>111</v>
       </c>
       <c r="D83" s="2" t="s">
         <v>12</v>
@@ -2574,7 +2729,7 @@
     </row>
     <row r="84" spans="1:11" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
@@ -2586,43 +2741,43 @@
       <c r="J84" s="20"/>
       <c r="K84" s="20"/>
     </row>
-    <row r="85" spans="1:11" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
-        <v>166</v>
+        <v>261</v>
       </c>
       <c r="B85" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>48</v>
+        <v>114</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="86" spans="1:11" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>167</v>
+        <v>262</v>
       </c>
       <c r="B86" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>50</v>
+        <v>115</v>
       </c>
       <c r="D86" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="87" spans="1:11" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
-        <v>168</v>
+        <v>263</v>
       </c>
       <c r="B87" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>52</v>
+        <v>116</v>
       </c>
       <c r="D87" s="2" t="s">
         <v>9</v>
@@ -2630,13 +2785,13 @@
     </row>
     <row r="88" spans="1:11" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
-        <v>158</v>
+        <v>264</v>
       </c>
       <c r="B88" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>53</v>
+        <v>117</v>
       </c>
       <c r="D88" s="2" t="s">
         <v>10</v>
@@ -2644,69 +2799,69 @@
     </row>
     <row r="89" spans="1:11" ht="87" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
-        <v>169</v>
+        <v>265</v>
       </c>
       <c r="B89" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>54</v>
+        <v>118</v>
       </c>
       <c r="D89" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="90" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>170</v>
+        <v>266</v>
       </c>
       <c r="B90" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>49</v>
+        <v>119</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="91" spans="1:11" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>171</v>
+        <v>267</v>
       </c>
       <c r="B91" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>51</v>
+        <v>120</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
     </row>
     <row r="92" spans="1:11" ht="63" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
-        <v>159</v>
+        <v>268</v>
       </c>
       <c r="B92" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>48</v>
+        <v>114</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
     </row>
     <row r="93" spans="1:11" ht="63" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
-        <v>160</v>
+        <v>269</v>
       </c>
       <c r="B93" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>50</v>
+        <v>115</v>
       </c>
       <c r="D93" s="2" t="s">
         <v>7</v>
@@ -2714,13 +2869,13 @@
     </row>
     <row r="94" spans="1:11" ht="63" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
-        <v>161</v>
+        <v>270</v>
       </c>
       <c r="B94" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>52</v>
+        <v>116</v>
       </c>
       <c r="D94" s="2" t="s">
         <v>9</v>
@@ -2728,13 +2883,13 @@
     </row>
     <row r="95" spans="1:11" ht="63" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
-        <v>162</v>
+        <v>271</v>
       </c>
       <c r="B95" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>53</v>
+        <v>117</v>
       </c>
       <c r="D95" s="2" t="s">
         <v>10</v>
@@ -2742,13 +2897,13 @@
     </row>
     <row r="96" spans="1:11" ht="63" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>163</v>
+        <v>272</v>
       </c>
       <c r="B96" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>54</v>
+        <v>118</v>
       </c>
       <c r="D96" s="2" t="s">
         <v>12</v>
@@ -2756,247 +2911,247 @@
     </row>
     <row r="97" spans="1:5" ht="63" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
-        <v>164</v>
+        <v>273</v>
       </c>
       <c r="B97" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>49</v>
+        <v>119</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="63" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>165</v>
+        <v>274</v>
       </c>
       <c r="B98" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>51</v>
+        <v>120</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
     </row>
     <row r="99" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>181</v>
+        <v>34</v>
       </c>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
       <c r="D99" s="2"/>
     </row>
-    <row r="100" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
-        <v>201</v>
+        <v>275</v>
       </c>
       <c r="B100" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>182</v>
+        <v>121</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
-        <v>202</v>
+        <v>276</v>
       </c>
       <c r="B101" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>183</v>
+        <v>122</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E101" s="9"/>
     </row>
-    <row r="102" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
-        <v>203</v>
+        <v>277</v>
       </c>
       <c r="B102" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>184</v>
+        <v>123</v>
       </c>
       <c r="D102" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="103" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
-        <v>204</v>
+        <v>278</v>
       </c>
       <c r="B103" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>185</v>
+        <v>124</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
-        <v>205</v>
+        <v>279</v>
       </c>
       <c r="B104" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>186</v>
+        <v>125</v>
       </c>
       <c r="D104" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="105" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
-        <v>206</v>
+        <v>280</v>
       </c>
       <c r="B105" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>187</v>
+        <v>126</v>
       </c>
       <c r="D105" s="8" t="s">
         <v>7</v>
       </c>
       <c r="E105" s="10"/>
     </row>
-    <row r="106" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
-        <v>207</v>
+        <v>281</v>
       </c>
       <c r="B106" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>188</v>
+        <v>127</v>
       </c>
       <c r="D106" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="107" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
-        <v>208</v>
+        <v>282</v>
       </c>
       <c r="B107" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>189</v>
+        <v>128</v>
       </c>
       <c r="D107" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="108" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
-        <v>211</v>
+        <v>283</v>
       </c>
       <c r="B108" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>212</v>
+        <v>129</v>
       </c>
       <c r="D108" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="109" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
-        <v>172</v>
+        <v>284</v>
       </c>
       <c r="B109" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>182</v>
+        <v>121</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" ht="78.75" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
-        <v>173</v>
+        <v>285</v>
       </c>
       <c r="B110" s="23" t="s">
-        <v>180</v>
+        <v>33</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>183</v>
+        <v>122</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
-        <v>174</v>
+        <v>286</v>
       </c>
       <c r="B111" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>184</v>
+        <v>123</v>
       </c>
       <c r="D111" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="112" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
-        <v>175</v>
+        <v>287</v>
       </c>
       <c r="B112" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>185</v>
+        <v>124</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" ht="63" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
-        <v>176</v>
+        <v>288</v>
       </c>
       <c r="B113" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>186</v>
+        <v>125</v>
       </c>
       <c r="D113" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="114" spans="1:4" ht="63" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
-        <v>177</v>
+        <v>289</v>
       </c>
       <c r="B114" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>187</v>
+        <v>126</v>
       </c>
       <c r="D114" s="2" t="s">
         <v>7</v>
@@ -3004,119 +3159,119 @@
     </row>
     <row r="115" spans="1:4" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
-        <v>178</v>
+        <v>290</v>
       </c>
       <c r="B115" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>188</v>
+        <v>127</v>
       </c>
       <c r="D115" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="116" spans="1:4" ht="63" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
-        <v>179</v>
+        <v>291</v>
       </c>
       <c r="B116" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>189</v>
+        <v>128</v>
       </c>
       <c r="D116" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="117" spans="1:4" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
-        <v>209</v>
+        <v>292</v>
       </c>
       <c r="B117" s="23" t="s">
-        <v>180</v>
+        <v>33</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>210</v>
+        <v>130</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" ht="94.5" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
-        <v>224</v>
+        <v>293</v>
       </c>
       <c r="B118" s="23" t="s">
-        <v>180</v>
+        <v>33</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>213</v>
+        <v>131</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" ht="94.5" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
-        <v>223</v>
+        <v>294</v>
       </c>
       <c r="B119" s="23" t="s">
-        <v>180</v>
+        <v>33</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>214</v>
+        <v>132</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" ht="94.5" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
-        <v>220</v>
+        <v>295</v>
       </c>
       <c r="B120" s="23" t="s">
-        <v>180</v>
+        <v>33</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>219</v>
+        <v>133</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>227</v>
+        <v>42</v>
       </c>
     </row>
     <row r="121" spans="1:4" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
-        <v>221</v>
+        <v>296</v>
       </c>
       <c r="B121" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>213</v>
+        <v>131</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>217</v>
+        <v>38</v>
       </c>
     </row>
     <row r="122" spans="1:4" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
-        <v>222</v>
+        <v>297</v>
       </c>
       <c r="B122" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>214</v>
+        <v>132</v>
       </c>
       <c r="D122" s="2" t="s">
-        <v>218</v>
+        <v>39</v>
       </c>
     </row>
     <row r="123" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>190</v>
+        <v>35</v>
       </c>
       <c r="B123" s="2"/>
       <c r="C123" s="2"/>
@@ -3124,27 +3279,27 @@
     </row>
     <row r="124" spans="1:4" ht="63" x14ac:dyDescent="0.25">
       <c r="A124" s="3" t="s">
-        <v>228</v>
+        <v>298</v>
       </c>
       <c r="B124" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>191</v>
+        <v>134</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
     </row>
     <row r="125" spans="1:4" ht="63" x14ac:dyDescent="0.25">
       <c r="A125" s="3" t="s">
-        <v>239</v>
+        <v>148</v>
       </c>
       <c r="B125" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>192</v>
+        <v>135</v>
       </c>
       <c r="D125" s="2" t="s">
         <v>7</v>
@@ -3152,13 +3307,13 @@
     </row>
     <row r="126" spans="1:4" ht="63" x14ac:dyDescent="0.25">
       <c r="A126" s="3" t="s">
-        <v>240</v>
+        <v>146</v>
       </c>
       <c r="B126" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>193</v>
+        <v>136</v>
       </c>
       <c r="D126" s="2" t="s">
         <v>9</v>
@@ -3166,27 +3321,27 @@
     </row>
     <row r="127" spans="1:4" ht="63" x14ac:dyDescent="0.25">
       <c r="A127" s="3" t="s">
-        <v>241</v>
+        <v>145</v>
       </c>
       <c r="B127" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>194</v>
+        <v>137</v>
       </c>
       <c r="D127" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="128" spans="1:4" ht="63" x14ac:dyDescent="0.25">
       <c r="A128" s="3" t="s">
-        <v>242</v>
+        <v>147</v>
       </c>
       <c r="B128" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>195</v>
+        <v>138</v>
       </c>
       <c r="D128" s="2" t="s">
         <v>11</v>
@@ -3194,13 +3349,13 @@
     </row>
     <row r="129" spans="1:4" ht="63" x14ac:dyDescent="0.25">
       <c r="A129" s="3" t="s">
-        <v>243</v>
+        <v>149</v>
       </c>
       <c r="B129" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>196</v>
+        <v>139</v>
       </c>
       <c r="D129" s="2" t="s">
         <v>12</v>
@@ -3208,13 +3363,13 @@
     </row>
     <row r="130" spans="1:4" ht="63" x14ac:dyDescent="0.25">
       <c r="A130" s="3" t="s">
-        <v>244</v>
+        <v>150</v>
       </c>
       <c r="B130" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>197</v>
+        <v>140</v>
       </c>
       <c r="D130" s="2" t="s">
         <v>10</v>
@@ -3222,13 +3377,13 @@
     </row>
     <row r="131" spans="1:4" ht="63" x14ac:dyDescent="0.25">
       <c r="A131" s="3" t="s">
-        <v>245</v>
+        <v>151</v>
       </c>
       <c r="B131" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>198</v>
+        <v>141</v>
       </c>
       <c r="D131" s="2" t="s">
         <v>9</v>
@@ -3236,27 +3391,27 @@
     </row>
     <row r="132" spans="1:4" ht="63" x14ac:dyDescent="0.25">
       <c r="A132" s="3" t="s">
-        <v>246</v>
+        <v>152</v>
       </c>
       <c r="B132" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>199</v>
+        <v>142</v>
       </c>
       <c r="D132" s="2" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
     </row>
     <row r="133" spans="1:4" ht="63" x14ac:dyDescent="0.25">
       <c r="A133" s="3" t="s">
-        <v>247</v>
+        <v>153</v>
       </c>
       <c r="B133" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>200</v>
+        <v>143</v>
       </c>
       <c r="D133" s="2" t="s">
         <v>8</v>
@@ -3264,27 +3419,27 @@
     </row>
     <row r="134" spans="1:4" ht="63" x14ac:dyDescent="0.25">
       <c r="A134" s="3" t="s">
-        <v>229</v>
+        <v>154</v>
       </c>
       <c r="B134" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>191</v>
+        <v>134</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
     </row>
     <row r="135" spans="1:4" ht="63" x14ac:dyDescent="0.25">
       <c r="A135" s="3" t="s">
-        <v>230</v>
+        <v>155</v>
       </c>
       <c r="B135" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>192</v>
+        <v>135</v>
       </c>
       <c r="D135" s="2" t="s">
         <v>7</v>
@@ -3292,13 +3447,13 @@
     </row>
     <row r="136" spans="1:4" ht="63" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="s">
-        <v>231</v>
+        <v>156</v>
       </c>
       <c r="B136" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>193</v>
+        <v>136</v>
       </c>
       <c r="D136" s="2" t="s">
         <v>9</v>
@@ -3306,27 +3461,27 @@
     </row>
     <row r="137" spans="1:4" ht="63" x14ac:dyDescent="0.25">
       <c r="A137" s="3" t="s">
-        <v>232</v>
+        <v>157</v>
       </c>
       <c r="B137" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>194</v>
+        <v>137</v>
       </c>
       <c r="D137" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="138" spans="1:4" ht="63" x14ac:dyDescent="0.25">
       <c r="A138" s="3" t="s">
-        <v>233</v>
+        <v>158</v>
       </c>
       <c r="B138" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>195</v>
+        <v>138</v>
       </c>
       <c r="D138" s="2" t="s">
         <v>11</v>
@@ -3334,13 +3489,13 @@
     </row>
     <row r="139" spans="1:4" ht="63" x14ac:dyDescent="0.25">
       <c r="A139" s="3" t="s">
-        <v>234</v>
+        <v>159</v>
       </c>
       <c r="B139" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>196</v>
+        <v>139</v>
       </c>
       <c r="D139" s="2" t="s">
         <v>12</v>
@@ -3348,13 +3503,13 @@
     </row>
     <row r="140" spans="1:4" ht="63" x14ac:dyDescent="0.25">
       <c r="A140" s="3" t="s">
-        <v>235</v>
+        <v>160</v>
       </c>
       <c r="B140" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>197</v>
+        <v>140</v>
       </c>
       <c r="D140" s="2" t="s">
         <v>10</v>
@@ -3362,13 +3517,13 @@
     </row>
     <row r="141" spans="1:4" ht="63" x14ac:dyDescent="0.25">
       <c r="A141" s="3" t="s">
-        <v>236</v>
+        <v>161</v>
       </c>
       <c r="B141" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>198</v>
+        <v>141</v>
       </c>
       <c r="D141" s="2" t="s">
         <v>9</v>
@@ -3376,30 +3531,326 @@
     </row>
     <row r="142" spans="1:4" ht="63" x14ac:dyDescent="0.25">
       <c r="A142" s="3" t="s">
-        <v>237</v>
+        <v>162</v>
       </c>
       <c r="B142" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>199</v>
+        <v>142</v>
       </c>
       <c r="D142" s="2" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
     </row>
     <row r="143" spans="1:4" ht="63" x14ac:dyDescent="0.25">
       <c r="A143" s="3" t="s">
-        <v>238</v>
+        <v>163</v>
       </c>
       <c r="B143" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>200</v>
+        <v>143</v>
       </c>
       <c r="D143" s="2" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A144" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B144" s="2"/>
+      <c r="C144" s="2"/>
+      <c r="D144" s="2"/>
+    </row>
+    <row r="145" spans="1:4" ht="63" x14ac:dyDescent="0.25">
+      <c r="A145" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="B145" s="5"/>
+      <c r="C145" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D145" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" ht="63" x14ac:dyDescent="0.25">
+      <c r="A146" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B146" s="5"/>
+      <c r="C146" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="D146" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" ht="63" x14ac:dyDescent="0.25">
+      <c r="A147" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="B147" s="5"/>
+      <c r="C147" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="D147" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" ht="63" x14ac:dyDescent="0.25">
+      <c r="A148" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="B148" s="5"/>
+      <c r="C148" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="D148" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" ht="63" x14ac:dyDescent="0.25">
+      <c r="A149" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="B149" s="5"/>
+      <c r="C149" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D149" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" ht="63" x14ac:dyDescent="0.25">
+      <c r="A150" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="B150" s="5"/>
+      <c r="C150" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="D150" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" ht="63" x14ac:dyDescent="0.25">
+      <c r="A151" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="B151" s="5"/>
+      <c r="C151" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="D151" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" ht="63" x14ac:dyDescent="0.25">
+      <c r="A152" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="B152" s="5"/>
+      <c r="C152" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D152" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" ht="63" x14ac:dyDescent="0.25">
+      <c r="A153" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="B153" s="5"/>
+      <c r="C153" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="D153" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" ht="63" x14ac:dyDescent="0.25">
+      <c r="A154" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B154" s="5"/>
+      <c r="C154" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="D154" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" ht="63" x14ac:dyDescent="0.25">
+      <c r="A155" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B155" s="5"/>
+      <c r="C155" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="D155" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" ht="63" x14ac:dyDescent="0.25">
+      <c r="A156" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="B156" s="5"/>
+      <c r="C156" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="D156" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" ht="63" x14ac:dyDescent="0.25">
+      <c r="A157" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="B157" s="5"/>
+      <c r="C157" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="D157" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" ht="63" x14ac:dyDescent="0.25">
+      <c r="A158" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="B158" s="5"/>
+      <c r="C158" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="D158" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" ht="63" x14ac:dyDescent="0.25">
+      <c r="A159" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="B159" s="5"/>
+      <c r="C159" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="D159" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" ht="63" x14ac:dyDescent="0.25">
+      <c r="A160" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="B160" s="5"/>
+      <c r="C160" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="D160" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" ht="63" x14ac:dyDescent="0.25">
+      <c r="A161" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="B161" s="5"/>
+      <c r="C161" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="D161" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" ht="63" x14ac:dyDescent="0.25">
+      <c r="A162" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="B162" s="5"/>
+      <c r="C162" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="D162" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" ht="63" x14ac:dyDescent="0.25">
+      <c r="A163" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="B163" s="5"/>
+      <c r="C163" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="D163" s="2" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" ht="63" x14ac:dyDescent="0.25">
+      <c r="A164" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="B164" s="5"/>
+      <c r="C164" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="D164" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" ht="63" x14ac:dyDescent="0.25">
+      <c r="A165" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="B165" s="5"/>
+      <c r="C165" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="D165" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" ht="63" x14ac:dyDescent="0.25">
+      <c r="A166" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="B166" s="5"/>
+      <c r="C166" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="D166" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" ht="63" x14ac:dyDescent="0.25">
+      <c r="A167" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="B167" s="5"/>
+      <c r="C167" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="D167" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" ht="63" x14ac:dyDescent="0.25">
+      <c r="A168" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="B168" s="5"/>
+      <c r="C168" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="D168" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>